<commit_message>
Agregar casos en caracterizacion
</commit_message>
<xml_diff>
--- a/ExtraClase/Trade_Off-EscenariosCalidad.xlsx
+++ b/ExtraClase/Trade_Off-EscenariosCalidad.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Arias Ramirez\OneDrive\Escritorio\U\2024-2\IS2\ExtraClase\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{79797BED-757C-4A0B-9482-5468A2FEC398}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{37717A45-3B5A-4217-BA99-52B13E1A886A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -49,7 +49,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="639" uniqueCount="312">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="574" uniqueCount="247">
   <si>
     <t>Trade off de QA</t>
   </si>
@@ -537,285 +537,84 @@
     <t xml:space="preserve">Total: </t>
   </si>
   <si>
-    <t>Se debe implementar autenticación multifactor para todas las cuentas de usuario.</t>
-  </si>
-  <si>
     <t>Las sesiones de usuario deben expirar automáticamente después de un período de inactividad.</t>
   </si>
   <si>
     <t>Los usuarios deben poder restablecer su contraseña solo a través de un proceso de autenticación seguro.</t>
   </si>
   <si>
-    <t>Los usuarios deben recibir notificaciones de seguridad cuando se detecta actividad sospechosa en sus cuentas.</t>
-  </si>
-  <si>
     <t>La contraseña debe cumplir con criterios de complejidad definidos por el sistema (longitud mínima, caracteres especiales, etc.).</t>
   </si>
   <si>
-    <t>Las contraseñas de los usuarios deben ser almacenadas utilizando técnicas de hashing seguras.</t>
-  </si>
-  <si>
-    <t>El sistema debe permitir la autenticación basada en tokens de acceso temporales y seguros.</t>
-  </si>
-  <si>
-    <t>Se debe aplicar un registro de auditoría detallado para todas las operaciones críticas realizadas por los usuarios.</t>
-  </si>
-  <si>
-    <t>Se deben implementar restricciones de acceso basadas en la ubicación geográfica del usuario.</t>
-  </si>
-  <si>
     <t>El sistema debe bloquear temporalmente la cuenta del usuario después de varios intentos fallidos de autenticación.</t>
   </si>
   <si>
     <t>Los administradores deben poder revocar el acceso de un usuario en cualquier momento.</t>
   </si>
   <si>
-    <t>Las políticas de contraseñas deben ser revisadas periódicamente y actualizadas según las mejores prácticas de seguridad.</t>
-  </si>
-  <si>
-    <t>Los usuarios deben recibir un aviso de seguridad si sus credenciales han sido comprometidas.</t>
-  </si>
-  <si>
     <t>El acceso a funciones administrativas debe estar restringido solo a usuarios autorizados.</t>
   </si>
   <si>
     <t>El sistema debe permitir a los usuarios revisar el historial de inicio de sesión y actividades recientes.</t>
   </si>
   <si>
-    <t>Los datos sensibles deben ser cifrados durante la transmisión y almacenamiento.</t>
-  </si>
-  <si>
-    <t>Los usuarios deben ser notificados de cualquier intento de acceso no autorizado a sus cuentas.</t>
-  </si>
-  <si>
-    <t>El sistema debe validar las entradas de los usuarios para prevenir ataques de inyección SQL y otros tipos de inyecciones.</t>
-  </si>
-  <si>
-    <t>Se debe implementar autenticación biométrica opcional para los usuarios que deseen mayor seguridad.</t>
-  </si>
-  <si>
     <t>Los usuarios deben tener la capacidad de establecer restricciones de tiempo para el acceso a sus cuentas.</t>
   </si>
   <si>
-    <t>El sistema debe permitir la autenticación a través de servicios de terceros seguros (por ejemplo, OAuth).</t>
-  </si>
-  <si>
-    <t>El acceso a las API del sistema debe estar limitado a través de autenticación con tokens API seguros.</t>
-  </si>
-  <si>
-    <t>Se debe implementar protección contra ataques de denegación de servicio (DoS).</t>
-  </si>
-  <si>
     <t>El sistema debe permitir a los usuarios configurar notificaciones de inicio de sesión desde nuevos dispositivos.</t>
   </si>
   <si>
-    <t>Todos los intentos de modificación de datos críticos deben ser aprobados por múltiples usuarios autorizados (autorización múltiple).</t>
-  </si>
-  <si>
-    <t>Se debe realizar un análisis de seguridad periódicamente para identificar y corregir vulnerabilidades.</t>
-  </si>
-  <si>
-    <t>Los usuarios deben poder reportar actividad sospechosa directamente desde el sistema.</t>
-  </si>
-  <si>
-    <t>El acceso a las funcionalidades críticas debe ser registrado y monitorizado en tiempo real.</t>
-  </si>
-  <si>
     <t>El sistema debe implementar mecanismos de recuperación segura en caso de incidentes de seguridad.</t>
   </si>
   <si>
-    <t>Todos los datos transmitidos entre el servidor y el cliente deben utilizar cifrado SSL/TLS.</t>
-  </si>
-  <si>
-    <t>El sistema debe tener una disponibilidad del 99.9% del tiempo para servicios críticos.</t>
-  </si>
-  <si>
     <t>Se debe implementar un sistema de recuperación automática que reinicie servicios en caso de fallos.</t>
   </si>
   <si>
     <t>El sistema debe realizar copias de seguridad automáticas cada 24 horas para minimizar la pérdida de datos.</t>
   </si>
   <si>
-    <t>Los usuarios deben poder acceder al sistema a través de múltiples servidores distribuidos geográficamente para mejorar la disponibilidad.</t>
-  </si>
-  <si>
     <t>El sistema debe contar con un plan de recuperación ante desastres que permita restaurar la funcionalidad completa en menos de 4 horas.</t>
   </si>
   <si>
-    <t>Se debe proporcionar acceso redundante al sistema a través de múltiples puntos de entrada (por ejemplo, aplicaciones móviles y web).</t>
-  </si>
-  <si>
-    <t>El sistema debe soportar la conmutación por error automática a servidores de respaldo en caso de interrupciones.</t>
-  </si>
-  <si>
-    <t>Se debe implementar un sistema de balanceo de carga para distribuir el tráfico y evitar sobrecargas en los servidores.</t>
-  </si>
-  <si>
-    <t>El sistema debe tener mecanismos para detectar y mitigar ataques DDoS que puedan afectar la disponibilidad.</t>
-  </si>
-  <si>
     <t>Los usuarios deben ser notificados proactivamente en caso de interrupciones planificadas o no planificadas.</t>
   </si>
   <si>
-    <t>Las actualizaciones del sistema deben realizarse con interrupciones mínimas o nulas en el servicio.</t>
-  </si>
-  <si>
-    <t>El sistema debe ser capaz de escalar automáticamente en respuesta a picos inesperados de tráfico.</t>
-  </si>
-  <si>
-    <t>Se debe contar con infraestructura en la nube que permita el rápido despliegue de recursos adicionales en caso de necesidad.</t>
-  </si>
-  <si>
-    <t>El sistema debe estar disponible en múltiples zonas de disponibilidad para garantizar la continuidad del servicio.</t>
-  </si>
-  <si>
-    <t>Se debe implementar un monitoreo en tiempo real del estado del sistema y alertas en caso de problemas de disponibilidad.</t>
-  </si>
-  <si>
     <t>El sistema debe permitir el acceso offline a funciones críticas en caso de pérdida de conectividad.</t>
   </si>
   <si>
-    <t>Las bases de datos deben tener réplicas en tiempo real para garantizar la continuidad del servicio en caso de fallos.</t>
-  </si>
-  <si>
-    <t>Se debe contar con un equipo de soporte técnico disponible 24/7 para responder a incidentes críticos de disponibilidad.</t>
-  </si>
-  <si>
     <t>El sistema debe estar diseñado para ser tolerante a fallos, permitiendo que las fallas parciales no afecten la disponibilidad total.</t>
   </si>
   <si>
-    <t>El sistema debe tener un tiempo de respuesta máximo de 2 segundos bajo carga nominal para garantizar una alta disponibilidad.</t>
-  </si>
-  <si>
-    <t>Se debe implementar una prueba de resistencia periódica para asegurar que el sistema puede manejar cargas máximas esperadas.</t>
-  </si>
-  <si>
-    <t>Los servidores de aplicaciones deben ser redundantes y distribuidos en varias ubicaciones geográficas.</t>
-  </si>
-  <si>
-    <t>Las actualizaciones críticas del sistema deben ser probadas en entornos simulados antes de su implementación en producción.</t>
-  </si>
-  <si>
-    <t>Se debe tener la capacidad de revertir actualizaciones que causen problemas de disponibilidad.</t>
-  </si>
-  <si>
-    <t>El sistema debe incluir un sistema de notificaciones automáticas para alertar a los administradores en caso de caída.</t>
-  </si>
-  <si>
-    <t>Las operaciones de mantenimiento deben ser planificadas y anunciadas con antelación para minimizar el impacto en la disponibilidad.</t>
-  </si>
-  <si>
-    <t>El sistema debe contar con energía de respaldo para evitar caídas debido a cortes de electricidad.</t>
-  </si>
-  <si>
-    <t>Se deben realizar pruebas de recuperación periódicas para asegurar que el sistema puede recuperarse rápidamente de un fallo.</t>
-  </si>
-  <si>
-    <t>El sistema debe poder operar en modo degradado, permitiendo el acceso a funciones esenciales si algunos servicios están inactivos.</t>
-  </si>
-  <si>
     <t>Se debe mantener un registro histórico de la disponibilidad del sistema para análisis y mejora continua.</t>
   </si>
   <si>
     <t>La aplicación debe ser compatible con versiones anteriores de los principales sistemas operativos.</t>
   </si>
   <si>
-    <t>La aplicación debe poder ejecutarse en dispositivos móviles con sistemas operativos Android e iOS.</t>
-  </si>
-  <si>
-    <t>La aplicación debe permitir la importación y exportación de datos en formatos estándar para facilitar la migración entre plataformas.</t>
-  </si>
-  <si>
-    <t>La aplicación debe ser fácil de trasladar a diferentes entornos de desarrollo y producción sin requerir modificaciones significativas.</t>
-  </si>
-  <si>
-    <t>La aplicación debe ser capaz de integrarse con una variedad de servicios y APIs de terceros en diferentes plataformas.</t>
-  </si>
-  <si>
-    <t>La aplicación debe estar empaquetada de forma que se pueda distribuir fácilmente a través de diferentes canales (App Store, repositorios, etc.).</t>
-  </si>
-  <si>
     <t>La aplicación debe ser compatible con arquitecturas de 32 y 64 bits en todos los sistemas operativos soportados.</t>
   </si>
   <si>
-    <t>La aplicación debe soportar la ejecución en entornos virtualizados y contenedorizados (por ejemplo, Docker).</t>
-  </si>
-  <si>
     <t>La aplicación debe tener un instalador que detecte automáticamente las configuraciones del sistema y ajuste la instalación en consecuencia.</t>
   </si>
   <si>
-    <t>La aplicación debe ser capaz de almacenar configuraciones específicas del sistema en archivos de configuración externos para facilitar la portabilidad.</t>
-  </si>
-  <si>
     <t>La aplicación debe estar diseñada para funcionar de manera eficiente en dispositivos con diferentes capacidades de hardware (por ejemplo, diferentes tamaños de memoria y velocidad de CPU).</t>
   </si>
   <si>
     <t>La aplicación debe soportar la localización y ser fácil de traducir a diferentes idiomas sin modificar el código fuente.</t>
   </si>
   <si>
-    <t>La aplicación debe poder ser desplegada en la nube, utilizando servicios de proveedores como AWS, Azure, y Google Cloud.</t>
-  </si>
-  <si>
     <t>La aplicación debe poder interactuar con sistemas de archivos de diferentes plataformas sin necesidad de conversión manual.</t>
   </si>
   <si>
-    <t>La aplicación debe ser capaz de adaptarse a las políticas de seguridad y configuración de diferentes entornos corporativos.</t>
-  </si>
-  <si>
     <t>La aplicación debe permitir actualizaciones y parches que no interrumpan su funcionamiento en diferentes sistemas operativos.</t>
   </si>
   <si>
-    <t>La aplicación debe proporcionar una interfaz de línea de comandos (CLI) que funcione en múltiples sistemas operativos.</t>
-  </si>
-  <si>
-    <t>La aplicación debe ser compatible con múltiples navegadores web en caso de tener una interfaz web.</t>
-  </si>
-  <si>
-    <t>La aplicación debe poder ejecutarse en versiones minimalistas de sistemas operativos, como las ediciones server sin interfaz gráfica.</t>
-  </si>
-  <si>
-    <t>La aplicación debe poder instalarse desde un medio físico, como un CD o USB, en caso de que no haya acceso a Internet.</t>
-  </si>
-  <si>
-    <t>La aplicación debe ser capaz de funcionar en sistemas con diferentes sistemas de archivos (por ejemplo, NTFS, ext4, APFS).</t>
-  </si>
-  <si>
-    <t>La aplicación debe soportar diferentes versiones de las principales dependencias y librerías de sistema.</t>
-  </si>
-  <si>
-    <t>La aplicación debe proporcionar un script de instalación multiplataforma para facilitar la implementación en diferentes entornos.</t>
-  </si>
-  <si>
     <t>La aplicación debe poder ser desinstalada completamente de cualquier sistema operativo sin dejar rastros innecesarios.</t>
   </si>
   <si>
-    <t>La aplicación debe soportar configuraciones de red variables, permitiendo la operación tanto en redes corporativas como domésticas.</t>
-  </si>
-  <si>
     <t>La aplicación debe estar optimizada para funcionar tanto en sistemas con pantallas táctiles como en sistemas tradicionales de teclado y ratón.</t>
   </si>
   <si>
-    <t>La aplicación debe poder integrarse con diferentes herramientas de desarrollo y CI/CD en múltiples plataformas.</t>
-  </si>
-  <si>
-    <t>La aplicación debe ser capaz de manejar diferentes codificaciones de caracteres (por ejemplo, UTF-8, ASCII) en diferentes sistemas operativos.</t>
-  </si>
-  <si>
-    <t>La aplicación debe permitir la configuración manual de rutas y variables de entorno para facilitar su portabilidad.</t>
-  </si>
-  <si>
-    <t>La aplicación debe estar documentada de manera que facilite a los desarrolladores la adaptación a nuevas plataformas y sistemas operativos.</t>
-  </si>
-  <si>
-    <t>El sistema debe ser capaz de procesar y almacenar 10,000 registros en menos de 5 segundos.</t>
-  </si>
-  <si>
-    <t>El sistema debe poder realizar búsquedas en bases de datos de 1 millón de registros en menos de 2 segundos.</t>
-  </si>
-  <si>
-    <t>El sistema debe optimizar el uso de la memoria para asegurar que no se superen los 500 MB durante la operación normal.</t>
-  </si>
-  <si>
     <t>El sistema debe realizar copias de seguridad incrementales en menos de 15 segundos.</t>
   </si>
   <si>
@@ -828,18 +627,6 @@
     <t>El sistema debe poder generar informes de uso en menos de 20 segundos.</t>
   </si>
   <si>
-    <t>El sistema debe soportar la concurrencia de 100 usuarios sin una degradación perceptible en el rendimiento.</t>
-  </si>
-  <si>
-    <t>El sistema debe poder realizar una sincronización de datos entre servidores en menos de 30 segundos.</t>
-  </si>
-  <si>
-    <t>El sistema debe inicializarse en menos de 10 segundos, incluso en configuraciones de hardware mínimas.</t>
-  </si>
-  <si>
-    <t>El sistema debe responder a solicitudes de la API en menos de 1 segundo bajo condiciones de carga nominal.</t>
-  </si>
-  <si>
     <t>El sistema debe ejecutar operaciones de actualización de software sin interrumpir el servicio por más de 5 segundos.</t>
   </si>
   <si>
@@ -852,9 +639,6 @@
     <t>El sistema debe optimizar el acceso a disco, reduciendo los tiempos de lectura/escritura a menos de 100 ms por operación.</t>
   </si>
   <si>
-    <t>El sistema debe poder realizar la validación de entradas en menos de 0.5 segundos.</t>
-  </si>
-  <si>
     <t>El sistema debe gestionar la transmisión de datos a través de la red manteniendo una latencia menor a 50 ms.</t>
   </si>
   <si>
@@ -985,6 +769,27 @@
   </si>
   <si>
     <t>La aplicación debe permitir la auditoría de los flujos de trabajo de aprobación, incluyendo quién aprueba qué y cuándo.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">El sistema debe solicitar una actualizacion en la contraseña cada cieto periodod de tiempo </t>
+  </si>
+  <si>
+    <t xml:space="preserve">si un usuario desea actualizar un diario requiere una aprovacion del otro propietario </t>
+  </si>
+  <si>
+    <t xml:space="preserve">los usuarios pueden reportar diredctamente errores o fallas desde el sistema </t>
+  </si>
+  <si>
+    <t>La aplicación debe permitir la exportación de datos en formatos estándar para facilitar la manipulacion.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">La aplicación debe de funcionar en multiples sistemas operativos como windows,macos  y linux </t>
+  </si>
+  <si>
+    <t>La aplicación debe poder instalarse desde un medio físico, como un CD o USB.</t>
+  </si>
+  <si>
+    <t>El sistema debe poder realizar la validación de entradas en menos de 3 segundos.</t>
   </si>
 </sst>
 </file>
@@ -1348,7 +1153,7 @@
     <xf numFmtId="0" fontId="4" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="54">
+  <cellXfs count="53">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -1436,6 +1241,16 @@
     <xf numFmtId="0" fontId="7" fillId="12" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="1" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="10" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="0" xfId="3" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="7" fillId="10" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -1471,17 +1286,6 @@
     </xf>
     <xf numFmtId="0" fontId="6" fillId="11" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="1" xfId="2" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="10" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="10" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="0" xfId="3" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="4">
@@ -3105,7 +2909,7 @@
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A2" s="47" t="s">
+      <c r="A2" s="35" t="s">
         <v>92</v>
       </c>
       <c r="B2" t="s">
@@ -3113,7 +2917,7 @@
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A3" s="47" t="s">
+      <c r="A3" s="35" t="s">
         <v>94</v>
       </c>
       <c r="B3" s="8" t="str">
@@ -3122,12 +2926,12 @@
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A4" s="47" t="s">
+      <c r="A4" s="35" t="s">
         <v>95</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A5" s="47" t="s">
+      <c r="A5" s="35" t="s">
         <v>96</v>
       </c>
     </row>
@@ -3188,7 +2992,7 @@
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A2" s="47" t="s">
+      <c r="A2" s="35" t="s">
         <v>92</v>
       </c>
       <c r="B2" t="s">
@@ -3196,7 +3000,7 @@
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A3" s="47" t="s">
+      <c r="A3" s="35" t="s">
         <v>94</v>
       </c>
       <c r="B3" s="8" t="str">
@@ -3205,12 +3009,12 @@
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A4" s="47" t="s">
+      <c r="A4" s="35" t="s">
         <v>95</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A5" s="47" t="s">
+      <c r="A5" s="35" t="s">
         <v>96</v>
       </c>
     </row>
@@ -3270,7 +3074,7 @@
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A2" s="47" t="s">
+      <c r="A2" s="35" t="s">
         <v>92</v>
       </c>
       <c r="B2" t="s">
@@ -3278,7 +3082,7 @@
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A3" s="47" t="s">
+      <c r="A3" s="35" t="s">
         <v>94</v>
       </c>
       <c r="B3" s="8" t="str">
@@ -3287,12 +3091,12 @@
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A4" s="47" t="s">
+      <c r="A4" s="35" t="s">
         <v>95</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A5" s="47" t="s">
+      <c r="A5" s="35" t="s">
         <v>96</v>
       </c>
     </row>
@@ -3339,74 +3143,74 @@
       <c r="A14" s="26" t="s">
         <v>104</v>
       </c>
-      <c r="B14" s="35" t="s">
+      <c r="B14" s="41" t="s">
         <v>105</v>
       </c>
-      <c r="C14" s="36"/>
-      <c r="D14" s="36"/>
-      <c r="E14" s="36"/>
-      <c r="F14" s="36"/>
-      <c r="G14" s="36"/>
-      <c r="H14" s="36"/>
-      <c r="I14" s="37"/>
+      <c r="C14" s="42"/>
+      <c r="D14" s="42"/>
+      <c r="E14" s="42"/>
+      <c r="F14" s="42"/>
+      <c r="G14" s="42"/>
+      <c r="H14" s="42"/>
+      <c r="I14" s="43"/>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A15" s="27" t="s">
         <v>106</v>
       </c>
-      <c r="B15" s="38" t="s">
+      <c r="B15" s="44" t="s">
         <v>107</v>
       </c>
-      <c r="C15" s="39"/>
-      <c r="D15" s="39"/>
-      <c r="E15" s="39"/>
-      <c r="F15" s="39"/>
-      <c r="G15" s="39"/>
-      <c r="H15" s="39"/>
-      <c r="I15" s="40"/>
+      <c r="C15" s="45"/>
+      <c r="D15" s="45"/>
+      <c r="E15" s="45"/>
+      <c r="F15" s="45"/>
+      <c r="G15" s="45"/>
+      <c r="H15" s="45"/>
+      <c r="I15" s="46"/>
     </row>
     <row r="16" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="27" t="s">
         <v>95</v>
       </c>
-      <c r="B16" s="41" t="s">
+      <c r="B16" s="47" t="s">
         <v>108</v>
       </c>
-      <c r="C16" s="42"/>
-      <c r="D16" s="42"/>
-      <c r="E16" s="42"/>
-      <c r="F16" s="42"/>
-      <c r="G16" s="42"/>
-      <c r="H16" s="42"/>
-      <c r="I16" s="43"/>
+      <c r="C16" s="48"/>
+      <c r="D16" s="48"/>
+      <c r="E16" s="48"/>
+      <c r="F16" s="48"/>
+      <c r="G16" s="48"/>
+      <c r="H16" s="48"/>
+      <c r="I16" s="49"/>
     </row>
     <row r="17" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="27" t="s">
         <v>109</v>
       </c>
-      <c r="B17" s="41" t="s">
+      <c r="B17" s="47" t="s">
         <v>110</v>
       </c>
-      <c r="C17" s="42"/>
-      <c r="D17" s="42"/>
-      <c r="E17" s="42"/>
-      <c r="F17" s="42"/>
-      <c r="G17" s="42"/>
-      <c r="H17" s="42"/>
-      <c r="I17" s="43"/>
+      <c r="C17" s="48"/>
+      <c r="D17" s="48"/>
+      <c r="E17" s="48"/>
+      <c r="F17" s="48"/>
+      <c r="G17" s="48"/>
+      <c r="H17" s="48"/>
+      <c r="I17" s="49"/>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A18" s="44" t="s">
+      <c r="A18" s="50" t="s">
         <v>111</v>
       </c>
-      <c r="B18" s="45"/>
-      <c r="C18" s="45"/>
-      <c r="D18" s="45"/>
-      <c r="E18" s="45"/>
-      <c r="F18" s="45"/>
-      <c r="G18" s="45"/>
-      <c r="H18" s="45"/>
-      <c r="I18" s="46"/>
+      <c r="B18" s="51"/>
+      <c r="C18" s="51"/>
+      <c r="D18" s="51"/>
+      <c r="E18" s="51"/>
+      <c r="F18" s="51"/>
+      <c r="G18" s="51"/>
+      <c r="H18" s="51"/>
+      <c r="I18" s="52"/>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A19" s="28" t="s">
@@ -3647,7 +3451,7 @@
         <f>SUM(B3:D3)</f>
         <v>39</v>
       </c>
-      <c r="F3" s="49">
+      <c r="F3" s="37">
         <f>E3/$E$16</f>
         <v>0.14285714285714285</v>
       </c>
@@ -3669,7 +3473,7 @@
         <f t="shared" ref="E4:E15" si="0">SUM(B4:D4)</f>
         <v>23</v>
       </c>
-      <c r="F4" s="49">
+      <c r="F4" s="37">
         <f t="shared" ref="F4:F15" si="1">E4/$E$16</f>
         <v>8.4249084249084255E-2</v>
       </c>
@@ -3691,7 +3495,7 @@
         <f t="shared" si="0"/>
         <v>22</v>
       </c>
-      <c r="F5" s="50">
+      <c r="F5" s="38">
         <f t="shared" si="1"/>
         <v>8.0586080586080591E-2</v>
       </c>
@@ -3713,7 +3517,7 @@
         <f t="shared" si="0"/>
         <v>34</v>
       </c>
-      <c r="F6" s="49">
+      <c r="F6" s="37">
         <f t="shared" si="1"/>
         <v>0.12454212454212454</v>
       </c>
@@ -3735,7 +3539,7 @@
         <f t="shared" si="0"/>
         <v>20</v>
       </c>
-      <c r="F7" s="50">
+      <c r="F7" s="38">
         <f t="shared" si="1"/>
         <v>7.3260073260073263E-2</v>
       </c>
@@ -3757,7 +3561,7 @@
         <f t="shared" si="0"/>
         <v>24</v>
       </c>
-      <c r="F8" s="49">
+      <c r="F8" s="37">
         <f t="shared" si="1"/>
         <v>8.7912087912087919E-2</v>
       </c>
@@ -3779,7 +3583,7 @@
         <f t="shared" si="0"/>
         <v>17</v>
       </c>
-      <c r="F9" s="50">
+      <c r="F9" s="38">
         <f t="shared" si="1"/>
         <v>6.2271062271062272E-2</v>
       </c>
@@ -3801,7 +3605,7 @@
         <f t="shared" si="0"/>
         <v>24</v>
       </c>
-      <c r="F10" s="49">
+      <c r="F10" s="37">
         <f t="shared" si="1"/>
         <v>8.7912087912087919E-2</v>
       </c>
@@ -3823,7 +3627,7 @@
         <f t="shared" si="0"/>
         <v>21</v>
       </c>
-      <c r="F11" s="50">
+      <c r="F11" s="38">
         <f t="shared" si="1"/>
         <v>7.6923076923076927E-2</v>
       </c>
@@ -3845,7 +3649,7 @@
         <f t="shared" si="0"/>
         <v>19</v>
       </c>
-      <c r="F12" s="50">
+      <c r="F12" s="38">
         <f t="shared" si="1"/>
         <v>6.95970695970696E-2</v>
       </c>
@@ -3867,7 +3671,7 @@
         <f t="shared" si="0"/>
         <v>16</v>
       </c>
-      <c r="F13" s="50">
+      <c r="F13" s="38">
         <f t="shared" si="1"/>
         <v>5.8608058608058608E-2</v>
       </c>
@@ -3889,7 +3693,7 @@
         <f t="shared" si="0"/>
         <v>7</v>
       </c>
-      <c r="F14" s="50">
+      <c r="F14" s="38">
         <f t="shared" si="1"/>
         <v>2.564102564102564E-2</v>
       </c>
@@ -3911,13 +3715,13 @@
         <f t="shared" si="0"/>
         <v>7</v>
       </c>
-      <c r="F15" s="50">
+      <c r="F15" s="38">
         <f t="shared" si="1"/>
         <v>2.564102564102564E-2</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A16" s="51" t="s">
+      <c r="A16" s="4" t="s">
         <v>161</v>
       </c>
       <c r="B16" s="2">
@@ -3936,7 +3740,7 @@
         <f t="shared" si="2"/>
         <v>273</v>
       </c>
-      <c r="F16" s="52">
+      <c r="F16" s="39">
         <f>E16/$E$16</f>
         <v>1</v>
       </c>
@@ -4264,8 +4068,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8A4C73B9-0AF9-4DE7-8A91-18F0737D3184}">
   <dimension ref="A1:I152"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A115" workbookViewId="0">
-      <selection activeCell="E97" sqref="E97"/>
+    <sheetView tabSelected="1" topLeftCell="A116" workbookViewId="0">
+      <selection activeCell="E126" sqref="E126"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4308,9 +4112,7 @@
       <c r="C3" s="24" t="s">
         <v>90</v>
       </c>
-      <c r="E3" s="10" t="s">
-        <v>162</v>
-      </c>
+      <c r="E3" s="10"/>
     </row>
     <row r="4" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A4" s="18" t="s">
@@ -4322,9 +4124,6 @@
       <c r="C4" s="24" t="s">
         <v>148</v>
       </c>
-      <c r="E4" s="10" t="s">
-        <v>163</v>
-      </c>
     </row>
     <row r="5" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A5" s="18" t="s">
@@ -4333,9 +4132,6 @@
       <c r="B5" s="13" t="s">
         <v>24</v>
       </c>
-      <c r="E5" s="10" t="s">
-        <v>164</v>
-      </c>
     </row>
     <row r="6" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A6" s="18" t="s">
@@ -4344,9 +4140,7 @@
       <c r="B6" s="13" t="s">
         <v>25</v>
       </c>
-      <c r="E6" s="10" t="s">
-        <v>165</v>
-      </c>
+      <c r="E6" s="10"/>
     </row>
     <row r="7" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A7" s="18" t="s">
@@ -4355,9 +4149,6 @@
       <c r="B7" s="14" t="s">
         <v>26</v>
       </c>
-      <c r="E7" s="10" t="s">
-        <v>166</v>
-      </c>
     </row>
     <row r="8" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A8" s="18" t="s">
@@ -4366,9 +4157,7 @@
       <c r="B8" s="14" t="s">
         <v>27</v>
       </c>
-      <c r="E8" s="10" t="s">
-        <v>167</v>
-      </c>
+      <c r="E8" s="10"/>
       <c r="G8" s="10"/>
       <c r="H8" s="10"/>
       <c r="I8" s="10"/>
@@ -4380,9 +4169,7 @@
       <c r="B9" s="14" t="s">
         <v>28</v>
       </c>
-      <c r="E9" s="10" t="s">
-        <v>168</v>
-      </c>
+      <c r="E9" s="10"/>
       <c r="G9" s="10"/>
       <c r="H9" s="10"/>
       <c r="I9" s="10"/>
@@ -4394,9 +4181,7 @@
       <c r="B10" s="14" t="s">
         <v>29</v>
       </c>
-      <c r="E10" s="10" t="s">
-        <v>169</v>
-      </c>
+      <c r="E10" s="10"/>
       <c r="G10" s="10"/>
       <c r="H10" s="10"/>
       <c r="I10" s="10"/>
@@ -4408,9 +4193,7 @@
       <c r="B11" s="15" t="s">
         <v>33</v>
       </c>
-      <c r="E11" s="10" t="s">
-        <v>170</v>
-      </c>
+      <c r="E11" s="10"/>
       <c r="G11" s="10"/>
       <c r="H11" s="10"/>
       <c r="I11" s="10"/>
@@ -4422,9 +4205,6 @@
       <c r="B12" s="15" t="s">
         <v>39</v>
       </c>
-      <c r="E12" s="10" t="s">
-        <v>171</v>
-      </c>
       <c r="G12" s="10"/>
       <c r="H12" s="10"/>
       <c r="I12" s="10"/>
@@ -4436,9 +4216,6 @@
       <c r="B13" s="15" t="s">
         <v>38</v>
       </c>
-      <c r="E13" s="10" t="s">
-        <v>172</v>
-      </c>
       <c r="G13" s="10"/>
       <c r="H13" s="10"/>
       <c r="I13" s="10"/>
@@ -4450,9 +4227,7 @@
       <c r="B14" s="15" t="s">
         <v>35</v>
       </c>
-      <c r="E14" s="10" t="s">
-        <v>173</v>
-      </c>
+      <c r="E14" s="10"/>
       <c r="G14" s="10"/>
       <c r="H14" s="10"/>
       <c r="I14" s="10"/>
@@ -4464,9 +4239,7 @@
       <c r="B15" s="15" t="s">
         <v>36</v>
       </c>
-      <c r="E15" s="10" t="s">
-        <v>174</v>
-      </c>
+      <c r="E15" s="10"/>
       <c r="G15" s="10"/>
       <c r="H15" s="10"/>
       <c r="I15" s="10"/>
@@ -4478,22 +4251,16 @@
       <c r="B16" s="15" t="s">
         <v>37</v>
       </c>
-      <c r="E16" s="10" t="s">
-        <v>175</v>
-      </c>
       <c r="G16" s="10"/>
       <c r="H16" s="10"/>
       <c r="I16" s="10"/>
     </row>
-    <row r="17" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" s="18" t="s">
         <v>6</v>
       </c>
       <c r="B17" s="17" t="s">
         <v>57</v>
-      </c>
-      <c r="E17" s="10" t="s">
-        <v>176</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
@@ -4503,9 +4270,7 @@
       <c r="B18" s="17" t="s">
         <v>58</v>
       </c>
-      <c r="E18" s="10" t="s">
-        <v>177</v>
-      </c>
+      <c r="E18" s="10"/>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" s="18" t="s">
@@ -4514,9 +4279,7 @@
       <c r="B19" s="16" t="s">
         <v>60</v>
       </c>
-      <c r="E19" s="10" t="s">
-        <v>178</v>
-      </c>
+      <c r="E19" s="10"/>
     </row>
     <row r="20" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A20" s="18" t="s">
@@ -4525,9 +4288,7 @@
       <c r="B20" s="16" t="s">
         <v>34</v>
       </c>
-      <c r="E20" s="10" t="s">
-        <v>179</v>
-      </c>
+      <c r="E20" s="10"/>
     </row>
     <row r="21" spans="1:6" ht="60" x14ac:dyDescent="0.25">
       <c r="A21" s="18" t="s">
@@ -4536,9 +4297,7 @@
       <c r="B21" s="16" t="s">
         <v>83</v>
       </c>
-      <c r="E21" s="10" t="s">
-        <v>180</v>
-      </c>
+      <c r="E21" s="10"/>
     </row>
     <row r="22" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A22" s="18" t="s">
@@ -4547,9 +4306,6 @@
       <c r="B22" s="16" t="s">
         <v>84</v>
       </c>
-      <c r="E22" s="10" t="s">
-        <v>181</v>
-      </c>
     </row>
     <row r="23" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A23" s="18" t="s">
@@ -4558,35 +4314,31 @@
       <c r="B23" s="17" t="s">
         <v>89</v>
       </c>
-      <c r="E23" s="10" t="s">
-        <v>182</v>
-      </c>
-    </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="E23" s="10"/>
+    </row>
+    <row r="24" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A24" s="18" t="s">
         <v>6</v>
       </c>
-      <c r="B24" s="22"/>
-      <c r="E24" s="10" t="s">
-        <v>183</v>
-      </c>
-    </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B24" s="17" t="s">
+        <v>240</v>
+      </c>
+      <c r="E24" s="10"/>
+    </row>
+    <row r="25" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A25" s="18" t="s">
         <v>6</v>
       </c>
-      <c r="B25" s="22"/>
-      <c r="E25" s="10" t="s">
-        <v>184</v>
+      <c r="B25" s="40" t="s">
+        <v>164</v>
       </c>
     </row>
     <row r="26" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A26" s="18" t="s">
         <v>6</v>
       </c>
-      <c r="B26" s="22"/>
-      <c r="E26" s="10" t="s">
-        <v>185</v>
+      <c r="B26" s="40" t="s">
+        <v>165</v>
       </c>
       <c r="F26" s="11"/>
     </row>
@@ -4594,39 +4346,40 @@
       <c r="A27" s="18" t="s">
         <v>6</v>
       </c>
-      <c r="B27" s="22"/>
-      <c r="E27" s="10" t="s">
-        <v>186</v>
-      </c>
+      <c r="B27" s="40" t="s">
+        <v>166</v>
+      </c>
+      <c r="E27" s="10"/>
       <c r="F27" s="11"/>
     </row>
     <row r="28" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A28" s="18" t="s">
         <v>6</v>
       </c>
-      <c r="B28" s="22"/>
-      <c r="E28" s="10" t="s">
-        <v>187</v>
-      </c>
+      <c r="B28" s="40" t="s">
+        <v>162</v>
+      </c>
+      <c r="E28" s="10"/>
       <c r="F28" s="11"/>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A29" s="18" t="s">
         <v>6</v>
       </c>
-      <c r="B29" s="22"/>
-      <c r="E29" s="10" t="s">
-        <v>188</v>
+      <c r="B29" s="40" t="s">
+        <v>163</v>
       </c>
       <c r="F29" s="11"/>
     </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A30" s="18" t="s">
         <v>6</v>
       </c>
-      <c r="B30" s="22"/>
-      <c r="E30" s="10" t="s">
-        <v>189</v>
+      <c r="B30" s="40" t="s">
+        <v>167</v>
+      </c>
+      <c r="E30" s="40" t="s">
+        <v>169</v>
       </c>
       <c r="F30" s="11"/>
     </row>
@@ -4634,19 +4387,23 @@
       <c r="A31" s="18" t="s">
         <v>6</v>
       </c>
-      <c r="B31" s="22"/>
-      <c r="E31" s="10" t="s">
-        <v>190</v>
+      <c r="B31" s="40" t="s">
+        <v>168</v>
+      </c>
+      <c r="E31" s="40" t="s">
+        <v>241</v>
       </c>
       <c r="F31" s="11"/>
     </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A32" s="18" t="s">
         <v>6</v>
       </c>
-      <c r="B32" s="22"/>
-      <c r="E32" s="10" t="s">
-        <v>191</v>
+      <c r="B32" s="40" t="s">
+        <v>170</v>
+      </c>
+      <c r="E32" s="40" t="s">
+        <v>171</v>
       </c>
       <c r="F32" s="11"/>
     </row>
@@ -4654,15 +4411,13 @@
       <c r="A33" s="19" t="s">
         <v>2</v>
       </c>
-      <c r="B33" s="48" t="s">
+      <c r="B33" s="36" t="s">
         <v>160</v>
       </c>
       <c r="C33" s="24" t="s">
         <v>149</v>
       </c>
-      <c r="E33" s="10" t="s">
-        <v>192</v>
-      </c>
+      <c r="E33" s="10"/>
       <c r="F33" s="11"/>
     </row>
     <row r="34" spans="1:6" ht="45" x14ac:dyDescent="0.25">
@@ -4675,10 +4430,6 @@
       <c r="C34" s="24" t="s">
         <v>150</v>
       </c>
-      <c r="E34" s="10" t="s">
-        <v>193</v>
-      </c>
-      <c r="F34" s="11"/>
     </row>
     <row r="35" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A35" s="19" t="s">
@@ -4687,9 +4438,6 @@
       <c r="B35" s="17" t="s">
         <v>40</v>
       </c>
-      <c r="E35" s="10" t="s">
-        <v>194</v>
-      </c>
       <c r="F35" s="11"/>
     </row>
     <row r="36" spans="1:6" ht="45" x14ac:dyDescent="0.25">
@@ -4699,9 +4447,7 @@
       <c r="B36" s="17" t="s">
         <v>41</v>
       </c>
-      <c r="E36" s="10" t="s">
-        <v>195</v>
-      </c>
+      <c r="E36" s="10"/>
       <c r="F36" s="11"/>
     </row>
     <row r="37" spans="1:6" ht="45" x14ac:dyDescent="0.25">
@@ -4711,9 +4457,6 @@
       <c r="B37" s="17" t="s">
         <v>42</v>
       </c>
-      <c r="E37" s="10" t="s">
-        <v>196</v>
-      </c>
       <c r="F37" s="11"/>
     </row>
     <row r="38" spans="1:6" ht="45" x14ac:dyDescent="0.25">
@@ -4726,9 +4469,7 @@
       <c r="C38" s="7" t="s">
         <v>61</v>
       </c>
-      <c r="E38" s="10" t="s">
-        <v>197</v>
-      </c>
+      <c r="E38" s="10"/>
       <c r="F38" s="11"/>
     </row>
     <row r="39" spans="1:6" ht="45" x14ac:dyDescent="0.25">
@@ -4738,9 +4479,7 @@
       <c r="B39" s="17" t="s">
         <v>43</v>
       </c>
-      <c r="E39" s="10" t="s">
-        <v>198</v>
-      </c>
+      <c r="E39" s="10"/>
       <c r="F39" s="11"/>
     </row>
     <row r="40" spans="1:6" ht="30" x14ac:dyDescent="0.25">
@@ -4750,9 +4489,7 @@
       <c r="B40" s="17" t="s">
         <v>63</v>
       </c>
-      <c r="E40" s="10" t="s">
-        <v>199</v>
-      </c>
+      <c r="E40" s="10"/>
       <c r="F40" s="11"/>
     </row>
     <row r="41" spans="1:6" ht="30" x14ac:dyDescent="0.25">
@@ -4765,9 +4502,7 @@
       <c r="C41" s="7" t="s">
         <v>62</v>
       </c>
-      <c r="E41" s="10" t="s">
-        <v>200</v>
-      </c>
+      <c r="E41" s="10"/>
       <c r="F41" s="11"/>
     </row>
     <row r="42" spans="1:6" ht="45" x14ac:dyDescent="0.25">
@@ -4777,195 +4512,165 @@
       <c r="B42" s="17" t="s">
         <v>45</v>
       </c>
-      <c r="E42" s="10" t="s">
-        <v>201</v>
-      </c>
       <c r="F42" s="11"/>
     </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A43" s="19" t="s">
         <v>2</v>
       </c>
-      <c r="B43" s="22"/>
-      <c r="E43" s="10" t="s">
-        <v>202</v>
-      </c>
+      <c r="B43" s="16" t="s">
+        <v>242</v>
+      </c>
+      <c r="E43" s="10"/>
       <c r="F43" s="11"/>
     </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A44" s="19" t="s">
         <v>2</v>
       </c>
-      <c r="B44" s="22"/>
-      <c r="E44" s="10" t="s">
-        <v>203</v>
-      </c>
+      <c r="B44" s="16" t="s">
+        <v>172</v>
+      </c>
+      <c r="E44" s="10"/>
       <c r="F44" s="11"/>
     </row>
     <row r="45" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A45" s="19" t="s">
         <v>2</v>
       </c>
-      <c r="B45" s="22"/>
-      <c r="E45" s="10" t="s">
-        <v>204</v>
-      </c>
+      <c r="B45" s="16" t="s">
+        <v>173</v>
+      </c>
+      <c r="E45" s="10"/>
       <c r="F45" s="11"/>
     </row>
-    <row r="46" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A46" s="19" t="s">
         <v>2</v>
       </c>
-      <c r="B46" s="22"/>
-      <c r="E46" s="10" t="s">
-        <v>205</v>
-      </c>
+      <c r="B46" s="40" t="s">
+        <v>174</v>
+      </c>
+      <c r="E46" s="10"/>
       <c r="F46" s="11"/>
     </row>
     <row r="47" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A47" s="19" t="s">
         <v>2</v>
       </c>
-      <c r="B47" s="22"/>
-      <c r="E47" s="10" t="s">
-        <v>206</v>
-      </c>
+      <c r="B47" s="40" t="s">
+        <v>175</v>
+      </c>
+      <c r="E47" s="10"/>
       <c r="F47" s="11"/>
     </row>
-    <row r="48" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A48" s="19" t="s">
         <v>2</v>
       </c>
-      <c r="B48" s="22"/>
-      <c r="E48" s="10" t="s">
-        <v>207</v>
-      </c>
-    </row>
-    <row r="49" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="B48" s="40" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="49" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A49" s="19" t="s">
         <v>2</v>
       </c>
-      <c r="B49" s="22"/>
-      <c r="E49" s="10" t="s">
-        <v>208</v>
-      </c>
+      <c r="B49" s="40" t="s">
+        <v>177</v>
+      </c>
+      <c r="E49" s="10"/>
     </row>
     <row r="50" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A50" s="19" t="s">
         <v>2</v>
       </c>
-      <c r="B50" s="22"/>
-      <c r="E50" s="10" t="s">
-        <v>209</v>
-      </c>
-    </row>
-    <row r="51" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="B50" s="40" t="s">
+        <v>178</v>
+      </c>
+      <c r="E50" s="10"/>
+    </row>
+    <row r="51" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A51" s="19" t="s">
         <v>2</v>
       </c>
       <c r="B51" s="22"/>
-      <c r="E51" s="10" t="s">
-        <v>210</v>
-      </c>
-    </row>
-    <row r="52" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    </row>
+    <row r="52" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A52" s="19" t="s">
         <v>2</v>
       </c>
       <c r="B52" s="22"/>
-      <c r="E52" s="10" t="s">
-        <v>211</v>
-      </c>
-    </row>
-    <row r="53" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="E52" s="10"/>
+    </row>
+    <row r="53" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A53" s="19" t="s">
         <v>2</v>
       </c>
       <c r="B53" s="22"/>
-      <c r="E53" s="10" t="s">
-        <v>212</v>
-      </c>
-    </row>
-    <row r="54" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="E53" s="10"/>
+    </row>
+    <row r="54" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A54" s="19" t="s">
         <v>2</v>
       </c>
       <c r="B54" s="22"/>
-      <c r="E54" s="10" t="s">
-        <v>213</v>
-      </c>
-    </row>
-    <row r="55" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="E54" s="10"/>
+    </row>
+    <row r="55" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A55" s="19" t="s">
         <v>2</v>
       </c>
       <c r="B55" s="22"/>
-      <c r="E55" s="10" t="s">
-        <v>214</v>
-      </c>
+      <c r="E55" s="10"/>
     </row>
     <row r="56" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A56" s="19" t="s">
         <v>2</v>
       </c>
       <c r="B56" s="22"/>
-      <c r="E56" s="10" t="s">
-        <v>215</v>
-      </c>
-    </row>
-    <row r="57" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="E56" s="10"/>
+    </row>
+    <row r="57" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A57" s="19" t="s">
         <v>2</v>
       </c>
       <c r="B57" s="22"/>
-      <c r="E57" s="10" t="s">
-        <v>216</v>
-      </c>
-    </row>
-    <row r="58" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="E57" s="10"/>
+    </row>
+    <row r="58" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A58" s="19" t="s">
         <v>2</v>
       </c>
       <c r="B58" s="22"/>
-      <c r="E58" s="10" t="s">
-        <v>217</v>
-      </c>
+      <c r="E58" s="10"/>
     </row>
     <row r="59" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A59" s="19" t="s">
         <v>2</v>
       </c>
       <c r="B59" s="22"/>
-      <c r="E59" s="10" t="s">
-        <v>218</v>
-      </c>
-    </row>
-    <row r="60" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="E59" s="10"/>
+    </row>
+    <row r="60" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A60" s="19" t="s">
         <v>2</v>
       </c>
       <c r="B60" s="22"/>
-      <c r="E60" s="10" t="s">
-        <v>219</v>
-      </c>
-    </row>
-    <row r="61" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="E60" s="10"/>
+    </row>
+    <row r="61" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A61" s="19" t="s">
         <v>2</v>
       </c>
       <c r="B61" s="22"/>
-      <c r="E61" s="10" t="s">
-        <v>220</v>
-      </c>
-    </row>
-    <row r="62" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="E61" s="10"/>
+    </row>
+    <row r="62" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A62" s="19" t="s">
         <v>2</v>
       </c>
       <c r="B62" s="22"/>
-      <c r="E62" s="10" t="s">
-        <v>221</v>
-      </c>
     </row>
     <row r="63" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A63" s="20" t="s">
@@ -4977,9 +4682,6 @@
       <c r="C63" s="24" t="s">
         <v>151</v>
       </c>
-      <c r="E63" s="10" t="s">
-        <v>222</v>
-      </c>
     </row>
     <row r="64" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A64" s="20" t="s">
@@ -4991,9 +4693,6 @@
       <c r="C64" s="24" t="s">
         <v>152</v>
       </c>
-      <c r="E64" s="10" t="s">
-        <v>223</v>
-      </c>
     </row>
     <row r="65" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A65" s="20" t="s">
@@ -5002,9 +4701,6 @@
       <c r="B65" s="15" t="s">
         <v>48</v>
       </c>
-      <c r="E65" s="10" t="s">
-        <v>224</v>
-      </c>
     </row>
     <row r="66" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A66" s="20" t="s">
@@ -5013,9 +4709,7 @@
       <c r="B66" s="16" t="s">
         <v>49</v>
       </c>
-      <c r="E66" s="10" t="s">
-        <v>225</v>
-      </c>
+      <c r="E66" s="10"/>
     </row>
     <row r="67" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A67" s="20" t="s">
@@ -5024,9 +4718,7 @@
       <c r="B67" s="16" t="s">
         <v>50</v>
       </c>
-      <c r="E67" s="10" t="s">
-        <v>226</v>
-      </c>
+      <c r="E67" s="10"/>
     </row>
     <row r="68" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A68" s="20" t="s">
@@ -5038,9 +4730,7 @@
       <c r="C68" s="7" t="s">
         <v>65</v>
       </c>
-      <c r="E68" s="10" t="s">
-        <v>227</v>
-      </c>
+      <c r="E68" s="10"/>
     </row>
     <row r="69" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A69" s="20" t="s">
@@ -5052,83 +4742,83 @@
       <c r="C69" s="7" t="s">
         <v>66</v>
       </c>
-      <c r="E69" s="10" t="s">
-        <v>228</v>
-      </c>
-    </row>
-    <row r="70" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    </row>
+    <row r="70" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A70" s="20" t="s">
         <v>8</v>
       </c>
-      <c r="B70" s="22" t="s">
+      <c r="B70" s="17" t="s">
         <v>88</v>
       </c>
-      <c r="E70" s="10" t="s">
-        <v>229</v>
-      </c>
-    </row>
-    <row r="71" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="E70" s="10"/>
+    </row>
+    <row r="71" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A71" s="20" t="s">
         <v>8</v>
       </c>
-      <c r="B71" s="22"/>
-      <c r="E71" s="10" t="s">
-        <v>230</v>
+      <c r="B71" s="40" t="s">
+        <v>181</v>
       </c>
     </row>
     <row r="72" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A72" s="20" t="s">
         <v>8</v>
       </c>
-      <c r="B72" s="22"/>
-      <c r="E72" s="10" t="s">
-        <v>231</v>
-      </c>
+      <c r="B72" s="40" t="s">
+        <v>179</v>
+      </c>
+      <c r="E72" s="10"/>
     </row>
     <row r="73" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A73" s="20" t="s">
         <v>8</v>
       </c>
-      <c r="B73" s="22"/>
+      <c r="B73" s="40" t="s">
+        <v>180</v>
+      </c>
       <c r="E73" s="10" t="s">
-        <v>232</v>
+        <v>182</v>
       </c>
     </row>
     <row r="74" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A74" s="20" t="s">
         <v>8</v>
       </c>
-      <c r="B74" s="22"/>
+      <c r="B74" s="40" t="s">
+        <v>243</v>
+      </c>
       <c r="E74" s="10" t="s">
-        <v>233</v>
+        <v>183</v>
       </c>
     </row>
     <row r="75" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A75" s="20" t="s">
         <v>8</v>
       </c>
-      <c r="B75" s="22"/>
-      <c r="E75" s="10" t="s">
-        <v>234</v>
-      </c>
+      <c r="B75" s="17" t="s">
+        <v>244</v>
+      </c>
+      <c r="E75" s="10"/>
     </row>
     <row r="76" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A76" s="20" t="s">
         <v>8</v>
       </c>
-      <c r="B76" s="22"/>
+      <c r="B76" s="10" t="s">
+        <v>245</v>
+      </c>
       <c r="E76" s="10" t="s">
-        <v>235</v>
-      </c>
-    </row>
-    <row r="77" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="77" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A77" s="20" t="s">
         <v>8</v>
       </c>
-      <c r="B77" s="22"/>
-      <c r="E77" s="10" t="s">
-        <v>236</v>
-      </c>
+      <c r="B77" s="10" t="s">
+        <v>187</v>
+      </c>
+      <c r="E77" s="10"/>
     </row>
     <row r="78" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A78" s="20" t="s">
@@ -5136,71 +4826,56 @@
       </c>
       <c r="B78" s="22"/>
       <c r="E78" s="10" t="s">
-        <v>237</v>
-      </c>
-    </row>
-    <row r="79" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="79" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A79" s="20" t="s">
         <v>8</v>
       </c>
       <c r="B79" s="22"/>
-      <c r="E79" s="10" t="s">
-        <v>238</v>
-      </c>
-    </row>
-    <row r="80" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="E79" s="10"/>
+    </row>
+    <row r="80" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A80" s="20" t="s">
         <v>8</v>
       </c>
       <c r="B80" s="22"/>
-      <c r="E80" s="10" t="s">
-        <v>239</v>
-      </c>
-    </row>
-    <row r="81" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="E80" s="10"/>
+    </row>
+    <row r="81" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A81" s="20" t="s">
         <v>8</v>
       </c>
       <c r="B81" s="22"/>
-      <c r="E81" s="10" t="s">
-        <v>240</v>
-      </c>
-    </row>
-    <row r="82" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="E81" s="10"/>
+    </row>
+    <row r="82" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A82" s="20" t="s">
         <v>8</v>
       </c>
       <c r="B82" s="22"/>
-      <c r="E82" s="10" t="s">
-        <v>241</v>
-      </c>
-    </row>
-    <row r="83" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    </row>
+    <row r="83" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A83" s="20" t="s">
         <v>8</v>
       </c>
       <c r="B83" s="22"/>
-      <c r="E83" s="10" t="s">
-        <v>242</v>
-      </c>
-    </row>
-    <row r="84" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="E83" s="10"/>
+    </row>
+    <row r="84" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A84" s="20" t="s">
         <v>8</v>
       </c>
       <c r="B84" s="22"/>
-      <c r="E84" s="10" t="s">
-        <v>243</v>
-      </c>
-    </row>
-    <row r="85" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="E84" s="10"/>
+    </row>
+    <row r="85" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A85" s="20" t="s">
         <v>8</v>
       </c>
       <c r="B85" s="22"/>
-      <c r="E85" s="10" t="s">
-        <v>244</v>
-      </c>
+      <c r="E85" s="10"/>
     </row>
     <row r="86" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A86" s="20" t="s">
@@ -5208,62 +4883,49 @@
       </c>
       <c r="B86" s="22"/>
       <c r="E86" s="10" t="s">
-        <v>245</v>
-      </c>
-    </row>
-    <row r="87" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="87" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A87" s="20" t="s">
         <v>8</v>
       </c>
       <c r="B87" s="22"/>
-      <c r="E87" s="10" t="s">
-        <v>246</v>
-      </c>
-    </row>
-    <row r="88" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="E87" s="10"/>
+    </row>
+    <row r="88" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A88" s="20" t="s">
         <v>8</v>
       </c>
       <c r="B88" s="22"/>
-      <c r="E88" s="10" t="s">
-        <v>247</v>
-      </c>
-    </row>
-    <row r="89" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    </row>
+    <row r="89" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A89" s="20" t="s">
         <v>8</v>
       </c>
       <c r="B89" s="22"/>
-      <c r="E89" s="10" t="s">
-        <v>248</v>
-      </c>
-    </row>
-    <row r="90" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="E89" s="10"/>
+    </row>
+    <row r="90" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A90" s="20" t="s">
         <v>8</v>
       </c>
       <c r="B90" s="22"/>
-      <c r="E90" s="10" t="s">
-        <v>249</v>
-      </c>
-    </row>
-    <row r="91" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="E90" s="10"/>
+    </row>
+    <row r="91" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A91" s="20" t="s">
         <v>8</v>
       </c>
       <c r="B91" s="22"/>
-      <c r="E91" s="10" t="s">
-        <v>250</v>
-      </c>
-    </row>
-    <row r="92" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="E91" s="10"/>
+    </row>
+    <row r="92" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A92" s="20" t="s">
         <v>8</v>
       </c>
       <c r="B92" s="22"/>
-      <c r="E92" s="10" t="s">
-        <v>251</v>
-      </c>
+      <c r="E92" s="10"/>
     </row>
     <row r="93" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A93" s="21" t="s">
@@ -5275,9 +4937,7 @@
       <c r="C93" s="24" t="s">
         <v>153</v>
       </c>
-      <c r="E93" s="10" t="s">
-        <v>252</v>
-      </c>
+      <c r="E93" s="10"/>
     </row>
     <row r="94" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A94" s="21" t="s">
@@ -5289,9 +4949,7 @@
       <c r="C94" s="24" t="s">
         <v>154</v>
       </c>
-      <c r="E94" s="10" t="s">
-        <v>253</v>
-      </c>
+      <c r="E94" s="10"/>
     </row>
     <row r="95" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A95" s="21" t="s">
@@ -5300,9 +4958,7 @@
       <c r="B95" s="14" t="s">
         <v>31</v>
       </c>
-      <c r="E95" s="10" t="s">
-        <v>254</v>
-      </c>
+      <c r="E95" s="10"/>
     </row>
     <row r="96" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A96" s="21" t="s">
@@ -5312,7 +4968,7 @@
         <v>54</v>
       </c>
       <c r="E96" s="10" t="s">
-        <v>255</v>
+        <v>188</v>
       </c>
     </row>
     <row r="97" spans="1:5" ht="45" x14ac:dyDescent="0.25">
@@ -5322,8 +4978,8 @@
       <c r="B97" s="16" t="s">
         <v>55</v>
       </c>
-      <c r="E97" s="53" t="s">
-        <v>256</v>
+      <c r="E97" s="40" t="s">
+        <v>189</v>
       </c>
     </row>
     <row r="98" spans="1:5" ht="45" x14ac:dyDescent="0.25">
@@ -5334,7 +4990,7 @@
         <v>56</v>
       </c>
       <c r="E98" s="10" t="s">
-        <v>257</v>
+        <v>190</v>
       </c>
     </row>
     <row r="99" spans="1:5" ht="45" x14ac:dyDescent="0.25">
@@ -5345,19 +5001,17 @@
         <v>53</v>
       </c>
       <c r="E99" s="10" t="s">
-        <v>258</v>
-      </c>
-    </row>
-    <row r="100" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="100" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A100" s="21" t="s">
         <v>14</v>
       </c>
       <c r="B100" s="22" t="s">
         <v>86</v>
       </c>
-      <c r="E100" s="10" t="s">
-        <v>259</v>
-      </c>
+      <c r="E100" s="10"/>
     </row>
     <row r="101" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A101" s="21" t="s">
@@ -5366,27 +5020,25 @@
       <c r="B101" s="22" t="s">
         <v>87</v>
       </c>
-      <c r="E101" s="10" t="s">
-        <v>260</v>
-      </c>
+      <c r="E101" s="10"/>
     </row>
     <row r="102" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A102" s="21" t="s">
         <v>14</v>
       </c>
-      <c r="B102" s="22"/>
-      <c r="E102" s="10" t="s">
-        <v>261</v>
-      </c>
+      <c r="B102" s="10" t="s">
+        <v>193</v>
+      </c>
+      <c r="E102" s="10"/>
     </row>
     <row r="103" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A103" s="21" t="s">
         <v>14</v>
       </c>
-      <c r="B103" s="22"/>
-      <c r="E103" s="10" t="s">
-        <v>262</v>
-      </c>
+      <c r="B103" s="10" t="s">
+        <v>246</v>
+      </c>
+      <c r="E103" s="10"/>
     </row>
     <row r="104" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A104" s="21" t="s">
@@ -5394,7 +5046,7 @@
       </c>
       <c r="B104" s="22"/>
       <c r="E104" s="10" t="s">
-        <v>263</v>
+        <v>192</v>
       </c>
     </row>
     <row r="105" spans="1:5" x14ac:dyDescent="0.25">
@@ -5402,9 +5054,6 @@
         <v>14</v>
       </c>
       <c r="B105" s="22"/>
-      <c r="E105" s="10" t="s">
-        <v>264</v>
-      </c>
     </row>
     <row r="106" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A106" s="21" t="s">
@@ -5412,7 +5061,7 @@
       </c>
       <c r="B106" s="22"/>
       <c r="E106" s="10" t="s">
-        <v>265</v>
+        <v>194</v>
       </c>
     </row>
     <row r="107" spans="1:5" ht="30" x14ac:dyDescent="0.25">
@@ -5421,7 +5070,7 @@
       </c>
       <c r="B107" s="22"/>
       <c r="E107" s="10" t="s">
-        <v>266</v>
+        <v>195</v>
       </c>
     </row>
     <row r="108" spans="1:5" x14ac:dyDescent="0.25">
@@ -5429,9 +5078,6 @@
         <v>14</v>
       </c>
       <c r="B108" s="22"/>
-      <c r="E108" s="10" t="s">
-        <v>267</v>
-      </c>
     </row>
     <row r="109" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A109" s="21" t="s">
@@ -5439,7 +5085,7 @@
       </c>
       <c r="B109" s="22"/>
       <c r="E109" s="10" t="s">
-        <v>268</v>
+        <v>196</v>
       </c>
     </row>
     <row r="110" spans="1:5" x14ac:dyDescent="0.25">
@@ -5448,7 +5094,7 @@
       </c>
       <c r="B110" s="22"/>
       <c r="E110" s="10" t="s">
-        <v>269</v>
+        <v>197</v>
       </c>
     </row>
     <row r="111" spans="1:5" x14ac:dyDescent="0.25">
@@ -5457,7 +5103,7 @@
       </c>
       <c r="B111" s="22"/>
       <c r="E111" s="10" t="s">
-        <v>270</v>
+        <v>198</v>
       </c>
     </row>
     <row r="112" spans="1:5" ht="30" x14ac:dyDescent="0.25">
@@ -5466,7 +5112,7 @@
       </c>
       <c r="B112" s="22"/>
       <c r="E112" s="10" t="s">
-        <v>271</v>
+        <v>199</v>
       </c>
     </row>
     <row r="113" spans="1:5" ht="30" x14ac:dyDescent="0.25">
@@ -5475,7 +5121,7 @@
       </c>
       <c r="B113" s="22"/>
       <c r="E113" s="10" t="s">
-        <v>272</v>
+        <v>200</v>
       </c>
     </row>
     <row r="114" spans="1:5" ht="30" x14ac:dyDescent="0.25">
@@ -5484,7 +5130,7 @@
       </c>
       <c r="B114" s="22"/>
       <c r="E114" s="10" t="s">
-        <v>273</v>
+        <v>201</v>
       </c>
     </row>
     <row r="115" spans="1:5" ht="30" x14ac:dyDescent="0.25">
@@ -5493,7 +5139,7 @@
       </c>
       <c r="B115" s="22"/>
       <c r="E115" s="10" t="s">
-        <v>274</v>
+        <v>202</v>
       </c>
     </row>
     <row r="116" spans="1:5" ht="30" x14ac:dyDescent="0.25">
@@ -5502,7 +5148,7 @@
       </c>
       <c r="B116" s="22"/>
       <c r="E116" s="10" t="s">
-        <v>275</v>
+        <v>203</v>
       </c>
     </row>
     <row r="117" spans="1:5" ht="30" x14ac:dyDescent="0.25">
@@ -5511,7 +5157,7 @@
       </c>
       <c r="B117" s="22"/>
       <c r="E117" s="10" t="s">
-        <v>276</v>
+        <v>204</v>
       </c>
     </row>
     <row r="118" spans="1:5" x14ac:dyDescent="0.25">
@@ -5520,7 +5166,7 @@
       </c>
       <c r="B118" s="22"/>
       <c r="E118" s="10" t="s">
-        <v>277</v>
+        <v>205</v>
       </c>
     </row>
     <row r="119" spans="1:5" x14ac:dyDescent="0.25">
@@ -5529,7 +5175,7 @@
       </c>
       <c r="B119" s="22"/>
       <c r="E119" s="10" t="s">
-        <v>278</v>
+        <v>206</v>
       </c>
     </row>
     <row r="120" spans="1:5" ht="30" x14ac:dyDescent="0.25">
@@ -5538,7 +5184,7 @@
       </c>
       <c r="B120" s="22"/>
       <c r="E120" s="10" t="s">
-        <v>279</v>
+        <v>207</v>
       </c>
     </row>
     <row r="121" spans="1:5" x14ac:dyDescent="0.25">
@@ -5547,7 +5193,7 @@
       </c>
       <c r="B121" s="22"/>
       <c r="E121" s="10" t="s">
-        <v>280</v>
+        <v>208</v>
       </c>
     </row>
     <row r="122" spans="1:5" ht="30" x14ac:dyDescent="0.25">
@@ -5556,7 +5202,7 @@
       </c>
       <c r="B122" s="22"/>
       <c r="E122" s="10" t="s">
-        <v>281</v>
+        <v>209</v>
       </c>
     </row>
     <row r="123" spans="1:5" ht="45" x14ac:dyDescent="0.25">
@@ -5569,9 +5215,6 @@
       <c r="C123" s="24" t="s">
         <v>155</v>
       </c>
-      <c r="E123" s="10" t="s">
-        <v>282</v>
-      </c>
     </row>
     <row r="124" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A124" s="23" t="s">
@@ -5584,7 +5227,7 @@
         <v>156</v>
       </c>
       <c r="E124" s="10" t="s">
-        <v>283</v>
+        <v>211</v>
       </c>
     </row>
     <row r="125" spans="1:5" ht="45" x14ac:dyDescent="0.25">
@@ -5595,7 +5238,7 @@
         <v>69</v>
       </c>
       <c r="E125" s="10" t="s">
-        <v>284</v>
+        <v>212</v>
       </c>
     </row>
     <row r="126" spans="1:5" ht="30" x14ac:dyDescent="0.25">
@@ -5606,7 +5249,7 @@
         <v>70</v>
       </c>
       <c r="E126" s="10" t="s">
-        <v>285</v>
+        <v>213</v>
       </c>
     </row>
     <row r="127" spans="1:5" ht="45" x14ac:dyDescent="0.25">
@@ -5617,7 +5260,7 @@
         <v>72</v>
       </c>
       <c r="E127" s="10" t="s">
-        <v>286</v>
+        <v>214</v>
       </c>
     </row>
     <row r="128" spans="1:5" ht="30" x14ac:dyDescent="0.25">
@@ -5628,7 +5271,7 @@
         <v>74</v>
       </c>
       <c r="E128" s="10" t="s">
-        <v>287</v>
+        <v>215</v>
       </c>
     </row>
     <row r="129" spans="1:5" ht="45" x14ac:dyDescent="0.25">
@@ -5639,7 +5282,7 @@
         <v>75</v>
       </c>
       <c r="E129" s="10" t="s">
-        <v>288</v>
+        <v>216</v>
       </c>
     </row>
     <row r="130" spans="1:5" ht="30" x14ac:dyDescent="0.25">
@@ -5650,7 +5293,7 @@
         <v>76</v>
       </c>
       <c r="E130" s="10" t="s">
-        <v>289</v>
+        <v>217</v>
       </c>
     </row>
     <row r="131" spans="1:5" ht="45" x14ac:dyDescent="0.25">
@@ -5661,7 +5304,7 @@
         <v>78</v>
       </c>
       <c r="E131" s="10" t="s">
-        <v>290</v>
+        <v>218</v>
       </c>
     </row>
     <row r="132" spans="1:5" ht="45" x14ac:dyDescent="0.25">
@@ -5672,7 +5315,7 @@
         <v>79</v>
       </c>
       <c r="E132" s="10" t="s">
-        <v>291</v>
+        <v>219</v>
       </c>
     </row>
     <row r="133" spans="1:5" ht="45" x14ac:dyDescent="0.25">
@@ -5683,7 +5326,7 @@
         <v>77</v>
       </c>
       <c r="E133" s="10" t="s">
-        <v>292</v>
+        <v>220</v>
       </c>
     </row>
     <row r="134" spans="1:5" ht="45" x14ac:dyDescent="0.25">
@@ -5697,7 +5340,7 @@
         <v>85</v>
       </c>
       <c r="E134" s="10" t="s">
-        <v>293</v>
+        <v>221</v>
       </c>
     </row>
     <row r="135" spans="1:5" ht="30" x14ac:dyDescent="0.25">
@@ -5708,7 +5351,7 @@
         <v>81</v>
       </c>
       <c r="E135" s="10" t="s">
-        <v>294</v>
+        <v>222</v>
       </c>
     </row>
     <row r="136" spans="1:5" ht="45" x14ac:dyDescent="0.25">
@@ -5719,7 +5362,7 @@
         <v>82</v>
       </c>
       <c r="E136" s="10" t="s">
-        <v>295</v>
+        <v>223</v>
       </c>
     </row>
     <row r="137" spans="1:5" ht="30" x14ac:dyDescent="0.25">
@@ -5730,7 +5373,7 @@
         <v>71</v>
       </c>
       <c r="E137" s="10" t="s">
-        <v>296</v>
+        <v>224</v>
       </c>
     </row>
     <row r="138" spans="1:5" ht="45" x14ac:dyDescent="0.25">
@@ -5741,16 +5384,18 @@
         <v>73</v>
       </c>
       <c r="E138" s="10" t="s">
-        <v>297</v>
+        <v>225</v>
       </c>
     </row>
     <row r="139" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A139" s="23" t="s">
         <v>12</v>
       </c>
-      <c r="B139" s="22"/>
+      <c r="B139" s="10" t="s">
+        <v>210</v>
+      </c>
       <c r="E139" s="10" t="s">
-        <v>298</v>
+        <v>226</v>
       </c>
     </row>
     <row r="140" spans="1:5" ht="30" x14ac:dyDescent="0.25">
@@ -5759,7 +5404,7 @@
       </c>
       <c r="B140" s="22"/>
       <c r="E140" s="10" t="s">
-        <v>299</v>
+        <v>227</v>
       </c>
     </row>
     <row r="141" spans="1:5" ht="30" x14ac:dyDescent="0.25">
@@ -5768,7 +5413,7 @@
       </c>
       <c r="B141" s="22"/>
       <c r="E141" s="10" t="s">
-        <v>300</v>
+        <v>228</v>
       </c>
     </row>
     <row r="142" spans="1:5" ht="30" x14ac:dyDescent="0.25">
@@ -5777,7 +5422,7 @@
       </c>
       <c r="B142" s="22"/>
       <c r="E142" s="10" t="s">
-        <v>301</v>
+        <v>229</v>
       </c>
     </row>
     <row r="143" spans="1:5" ht="30" x14ac:dyDescent="0.25">
@@ -5786,7 +5431,7 @@
       </c>
       <c r="B143" s="22"/>
       <c r="E143" s="10" t="s">
-        <v>302</v>
+        <v>230</v>
       </c>
     </row>
     <row r="144" spans="1:5" ht="30" x14ac:dyDescent="0.25">
@@ -5795,7 +5440,7 @@
       </c>
       <c r="B144" s="22"/>
       <c r="E144" s="10" t="s">
-        <v>303</v>
+        <v>231</v>
       </c>
     </row>
     <row r="145" spans="1:5" ht="30" x14ac:dyDescent="0.25">
@@ -5804,7 +5449,7 @@
       </c>
       <c r="B145" s="22"/>
       <c r="E145" s="10" t="s">
-        <v>304</v>
+        <v>232</v>
       </c>
     </row>
     <row r="146" spans="1:5" ht="30" x14ac:dyDescent="0.25">
@@ -5813,7 +5458,7 @@
       </c>
       <c r="B146" s="22"/>
       <c r="E146" s="10" t="s">
-        <v>305</v>
+        <v>233</v>
       </c>
     </row>
     <row r="147" spans="1:5" ht="30" x14ac:dyDescent="0.25">
@@ -5822,7 +5467,7 @@
       </c>
       <c r="B147" s="22"/>
       <c r="E147" s="10" t="s">
-        <v>306</v>
+        <v>234</v>
       </c>
     </row>
     <row r="148" spans="1:5" ht="30" x14ac:dyDescent="0.25">
@@ -5831,7 +5476,7 @@
       </c>
       <c r="B148" s="22"/>
       <c r="E148" s="10" t="s">
-        <v>307</v>
+        <v>235</v>
       </c>
     </row>
     <row r="149" spans="1:5" ht="30" x14ac:dyDescent="0.25">
@@ -5840,7 +5485,7 @@
       </c>
       <c r="B149" s="22"/>
       <c r="E149" s="10" t="s">
-        <v>308</v>
+        <v>236</v>
       </c>
     </row>
     <row r="150" spans="1:5" ht="30" x14ac:dyDescent="0.25">
@@ -5849,7 +5494,7 @@
       </c>
       <c r="B150" s="22"/>
       <c r="E150" s="10" t="s">
-        <v>309</v>
+        <v>237</v>
       </c>
     </row>
     <row r="151" spans="1:5" ht="30" x14ac:dyDescent="0.25">
@@ -5858,7 +5503,7 @@
       </c>
       <c r="B151" s="22"/>
       <c r="E151" s="10" t="s">
-        <v>310</v>
+        <v>238</v>
       </c>
     </row>
     <row r="152" spans="1:5" ht="30" x14ac:dyDescent="0.25">
@@ -5867,7 +5512,7 @@
       </c>
       <c r="B152" s="22"/>
       <c r="E152" s="10" t="s">
-        <v>311</v>
+        <v>239</v>
       </c>
     </row>
   </sheetData>
@@ -5903,7 +5548,7 @@
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A2" s="47" t="s">
+      <c r="A2" s="35" t="s">
         <v>92</v>
       </c>
       <c r="B2" t="s">
@@ -5911,7 +5556,7 @@
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A3" s="47" t="s">
+      <c r="A3" s="35" t="s">
         <v>94</v>
       </c>
       <c r="B3" s="8" t="str">
@@ -5920,12 +5565,12 @@
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A4" s="47" t="s">
+      <c r="A4" s="35" t="s">
         <v>95</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A5" s="47" t="s">
+      <c r="A5" s="35" t="s">
         <v>96</v>
       </c>
     </row>
@@ -5985,7 +5630,7 @@
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A2" s="47" t="s">
+      <c r="A2" s="35" t="s">
         <v>92</v>
       </c>
       <c r="B2" t="s">
@@ -5993,7 +5638,7 @@
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A3" s="47" t="s">
+      <c r="A3" s="35" t="s">
         <v>94</v>
       </c>
       <c r="B3" s="8" t="str">
@@ -6002,12 +5647,12 @@
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A4" s="47" t="s">
+      <c r="A4" s="35" t="s">
         <v>95</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A5" s="47" t="s">
+      <c r="A5" s="35" t="s">
         <v>96</v>
       </c>
     </row>
@@ -6067,7 +5712,7 @@
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A2" s="47" t="s">
+      <c r="A2" s="35" t="s">
         <v>92</v>
       </c>
       <c r="B2" t="s">
@@ -6075,7 +5720,7 @@
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A3" s="47" t="s">
+      <c r="A3" s="35" t="s">
         <v>94</v>
       </c>
       <c r="B3" s="8" t="str">
@@ -6084,12 +5729,12 @@
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A4" s="47" t="s">
+      <c r="A4" s="35" t="s">
         <v>95</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A5" s="47" t="s">
+      <c r="A5" s="35" t="s">
         <v>96</v>
       </c>
     </row>
@@ -6149,7 +5794,7 @@
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A2" s="47" t="s">
+      <c r="A2" s="35" t="s">
         <v>92</v>
       </c>
       <c r="B2" t="s">
@@ -6157,7 +5802,7 @@
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A3" s="47" t="s">
+      <c r="A3" s="35" t="s">
         <v>94</v>
       </c>
       <c r="B3" s="8" t="str">
@@ -6166,12 +5811,12 @@
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A4" s="47" t="s">
+      <c r="A4" s="35" t="s">
         <v>95</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A5" s="47" t="s">
+      <c r="A5" s="35" t="s">
         <v>96</v>
       </c>
     </row>
@@ -6231,7 +5876,7 @@
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A2" s="47" t="s">
+      <c r="A2" s="35" t="s">
         <v>92</v>
       </c>
       <c r="B2" t="s">
@@ -6239,7 +5884,7 @@
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A3" s="47" t="s">
+      <c r="A3" s="35" t="s">
         <v>94</v>
       </c>
       <c r="B3" s="8" t="str">
@@ -6248,12 +5893,12 @@
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A4" s="47" t="s">
+      <c r="A4" s="35" t="s">
         <v>95</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A5" s="47" t="s">
+      <c r="A5" s="35" t="s">
         <v>96</v>
       </c>
     </row>
@@ -6313,7 +5958,7 @@
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A2" s="47" t="s">
+      <c r="A2" s="35" t="s">
         <v>92</v>
       </c>
       <c r="B2" t="s">
@@ -6321,7 +5966,7 @@
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A3" s="47" t="s">
+      <c r="A3" s="35" t="s">
         <v>94</v>
       </c>
       <c r="B3" s="8" t="str">
@@ -6330,12 +5975,12 @@
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A4" s="47" t="s">
+      <c r="A4" s="35" t="s">
         <v>95</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A5" s="47" t="s">
+      <c r="A5" s="35" t="s">
         <v>96</v>
       </c>
     </row>
@@ -6395,7 +6040,7 @@
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A2" s="47" t="s">
+      <c r="A2" s="35" t="s">
         <v>92</v>
       </c>
       <c r="B2" t="s">
@@ -6403,7 +6048,7 @@
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A3" s="47" t="s">
+      <c r="A3" s="35" t="s">
         <v>94</v>
       </c>
       <c r="B3" s="8" t="str">
@@ -6412,12 +6057,12 @@
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A4" s="47" t="s">
+      <c r="A4" s="35" t="s">
         <v>95</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A5" s="47" t="s">
+      <c r="A5" s="35" t="s">
         <v>96</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Añadir algunos escenarios de calidad
</commit_message>
<xml_diff>
--- a/ExtraClase/Trade_Off-EscenariosCalidad.xlsx
+++ b/ExtraClase/Trade_Off-EscenariosCalidad.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Arias Ramirez\OneDrive\Escritorio\U\2024-2\IS2\ExtraClase\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://uconet-my.sharepoint.com/personal/sergio_arias8941_uco_net_co/Documents/Desktop/Universidad/uco-2024-2/IS2/IS2/ExtraClase/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{37717A45-3B5A-4217-BA99-52B13E1A886A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="88" documentId="13_ncr:1_{37717A45-3B5A-4217-BA99-52B13E1A886A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{1C18233B-9673-4B5C-868D-0E45DD2BF723}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-60" yWindow="-60" windowWidth="20610" windowHeight="11040" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabla de Contenido" sheetId="1" r:id="rId1"/>
@@ -49,7 +49,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="574" uniqueCount="247">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="970" uniqueCount="425">
   <si>
     <t>Trade off de QA</t>
   </si>
@@ -684,12 +684,6 @@
     <t>La aplicación debe generar informes de auditoría automatizados que se puedan exportar en formatos estándar (como PDF o CSV).</t>
   </si>
   <si>
-    <t>La aplicación debe mantener registros de auditoría durante un período mínimo de 5 años para cumplir con normativas legales.</t>
-  </si>
-  <si>
-    <t>La aplicación debe permitir la auditoría de los accesos a la base de datos, incluyendo consultas y modificaciones de datos.</t>
-  </si>
-  <si>
     <t>La aplicación debe registrar y auditar todos los intentos de escalación de privilegios para detectar posibles amenazas.</t>
   </si>
   <si>
@@ -753,9 +747,6 @@
     <t>La aplicación debe mantener un registro detallado de todos los accesos y cambios en las configuraciones de red, incluyendo VPNs y proxies.</t>
   </si>
   <si>
-    <t>La aplicación debe permitir la auditoría de las políticas de retención y eliminación de datos, asegurando el cumplimiento de normativas.</t>
-  </si>
-  <si>
     <t>La aplicación debe registrar y auditar cualquier intento de modificación o eliminación de los registros de auditoría.</t>
   </si>
   <si>
@@ -790,6 +781,621 @@
   </si>
   <si>
     <t>El sistema debe poder realizar la validación de entradas en menos de 3 segundos.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Definir detalladamente </t>
+  </si>
+  <si>
+    <t xml:space="preserve">La aplicación no debe permitir la modificacion de los registros de auditoria </t>
+  </si>
+  <si>
+    <t xml:space="preserve">El sistema debe registrar un usuario en menos de 10 segundos </t>
+  </si>
+  <si>
+    <t xml:space="preserve">El sistema debe poder crar una nueva conversacion en menos de 10 segundos </t>
+  </si>
+  <si>
+    <t xml:space="preserve">El sistema debe poder registrar una invitacion en menos de 10 segundos </t>
+  </si>
+  <si>
+    <t xml:space="preserve">El sistema debe lleva r registro de todos los usuarios que intentan acceder o crear cuenta que no tengan autorisacion </t>
+  </si>
+  <si>
+    <t xml:space="preserve">El proceso de instalacion debe tardar menos de 5 minutos </t>
+  </si>
+  <si>
+    <t xml:space="preserve">El sistema debe de dar respuesta de si el usuario no registrado que intenta aceder cuenta con una invitacion o no esta autorisado en un tiempo menor a 5 segundos </t>
+  </si>
+  <si>
+    <t xml:space="preserve">El sistema debe de actualizar el estado de un mensaja una vez sea visto en un tiempo menor a 5 segundos </t>
+  </si>
+  <si>
+    <t xml:space="preserve">La aplicacion debe llevar registro de a quienes invita cada usuario y con que permisos fue la invitacion envidada </t>
+  </si>
+  <si>
+    <t xml:space="preserve">fin </t>
+  </si>
+  <si>
+    <t xml:space="preserve">extra </t>
+  </si>
+  <si>
+    <t>Se pueden degradar o bloquear el uso a los usuarios con roles inferiores</t>
+  </si>
+  <si>
+    <t>Cifrado de mensajes utilizando libretas de claves de un solo uso (OTP) y generadores de números aleatorios criptográficamente seguros (CSPRNG).</t>
+  </si>
+  <si>
+    <r>
+      <t>Característica:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> Cifrado de mensajes utilizando libretas de claves de un solo uso (OTP) y generadores de números aleatorios criptográficamente seguros (CSPRNG).</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Objetivo de negocio:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> Garantizar la confidencialidad absoluta de las comunicaciones, protegiéndolas contra cualquier intento de descifrado, incluso frente a amenazas futuras como la computación cuántica.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Descripción:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> Todos los mensajes deben ser cifrados utilizando libretas de claves de un solo uso (OTP) combinadas con generadores de números aleatorios criptográficamente seguros (CSPRNG), asegurando que no exista posibilidad de descifrado no autorizado.</t>
+    </r>
+  </si>
+  <si>
+    <t>Cuando un mensaje es enviado, debe ser cifrado automáticamente usando OTP y CSPRNG.</t>
+  </si>
+  <si>
+    <t>Envío de un mensaje</t>
+  </si>
+  <si>
+    <t>Sistema</t>
+  </si>
+  <si>
+    <t>Ambiente real de operación</t>
+  </si>
+  <si>
+    <t>El mensaje se cifra utilizando OTP y CSPRNG, garantizando su confidencialidad</t>
+  </si>
+  <si>
+    <t>Se ha comprobado que el mensaje está cifrado antes de ser enviado.</t>
+  </si>
+  <si>
+    <t>Si se intenta descifrar un mensaje sin la clave correcta, el sistema debe impedir el acceso al contenido.</t>
+  </si>
+  <si>
+    <t>Usuario malicioso</t>
+  </si>
+  <si>
+    <t>Intento de descifrado sin la clave correcta</t>
+  </si>
+  <si>
+    <t>Ambiente controlado de pruebas</t>
+  </si>
+  <si>
+    <t>El sistema rechaza el descifrado y mantiene el contenido inaccesible</t>
+  </si>
+  <si>
+    <t>Se ha comprobado que el mensaje no se descifra sin la clave correcta.</t>
+  </si>
+  <si>
+    <t>Cuando se recibe un mensaje cifrado, debe ser descifrado solo si la clave correcta está disponible en el dispositivo extraíble.</t>
+  </si>
+  <si>
+    <t>Recepción de un mensaje cifrado</t>
+  </si>
+  <si>
+    <t>El mensaje es descifrado solo si la clave correcta está disponible, asegurando su autenticidad</t>
+  </si>
+  <si>
+    <t>Se ha comprobado que el mensaje solo es accesible con la clave correcta.</t>
+  </si>
+  <si>
+    <t>Si se pierde la clave en el dispositivo extraíble, el mensaje debe permanecer inaccesible.</t>
+  </si>
+  <si>
+    <t>Pérdida de la clave</t>
+  </si>
+  <si>
+    <t>El mensaje permanece cifrado e inaccesible, garantizando la confidencialidad de los datos</t>
+  </si>
+  <si>
+    <t>Se ha comprobado que el mensaje no se puede descifrar sin la clave almacenada.</t>
+  </si>
+  <si>
+    <t>Cuando se genera un mensaje cifrado, debe cumplir con los estándares de criptografía avanzada.</t>
+  </si>
+  <si>
+    <t>Cifrado de un mensaje</t>
+  </si>
+  <si>
+    <t>Ambiente de desarrollo y pruebas</t>
+  </si>
+  <si>
+    <t>El mensaje cumple con los estándares establecidos, garantizando su seguridad a largo plazo</t>
+  </si>
+  <si>
+    <t>Se ha validado que el cifrado sigue las directrices de seguridad definidas.</t>
+  </si>
+  <si>
+    <t>Almacenamiento de claves criptográficas en dispositivos de almacenamiento extraíbles, como USBs.</t>
+  </si>
+  <si>
+    <r>
+      <t>Característica:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> Almacenamiento de claves criptográficas en dispositivos de almacenamiento extraíbles, como USBs.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Objetivo de negocio:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> Proteger las claves criptográficas de amenazas en línea, asegurando que solo los usuarios autorizados con acceso físico a los dispositivos puedan descifrar la información.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Descripción:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> Las claves criptográficas deben almacenarse en dispositivos extraíbles, lo que garantiza que permanezcan fuera de cualquier sistema conectado a la red, previniendo el acceso no autorizado.</t>
+    </r>
+  </si>
+  <si>
+    <t>Cuando se requiere descifrar un mensaje, el sistema debe solicitar la conexión del dispositivo USB con la clave criptográfica.</t>
+  </si>
+  <si>
+    <t>Solicitud de descifrado</t>
+  </si>
+  <si>
+    <t>El sistema pide la conexión del dispositivo USB con la clave para proceder con el descifrado</t>
+  </si>
+  <si>
+    <t>Se ha comprobado que el descifrado solo es posible con el dispositivo USB conectado.</t>
+  </si>
+  <si>
+    <t>Si el dispositivo USB es removido mientras el sistema está en uso, todas las operaciones criptográficas deben ser canceladas.</t>
+  </si>
+  <si>
+    <t>Remoción del dispositivo USB</t>
+  </si>
+  <si>
+    <t>Todas las operaciones criptográficas en curso son canceladas, protegiendo la confidencialidad de los datos</t>
+  </si>
+  <si>
+    <t>Se ha comprobado que las operaciones criptográficas se detienen al remover el USB.</t>
+  </si>
+  <si>
+    <t>Cuando un dispositivo USB con la clave criptográfica es conectado, el sistema debe autenticar el dispositivo antes de permitir su uso.</t>
+  </si>
+  <si>
+    <t>Conexión de un dispositivo USB con la clave</t>
+  </si>
+  <si>
+    <t>El sistema autentica el dispositivo antes de permitir cualquier operación con la clave</t>
+  </si>
+  <si>
+    <t>Se ha comprobado que el dispositivo USB es autenticado antes de su uso.</t>
+  </si>
+  <si>
+    <t>Si se intenta conectar un dispositivo USB no autorizado, el sistema debe rechazar su uso e informar al usuario.</t>
+  </si>
+  <si>
+    <t>Conexión de un dispositivo USB no autorizado</t>
+  </si>
+  <si>
+    <t>El sistema rechaza el uso del dispositivo no autorizado y notifica al usuario</t>
+  </si>
+  <si>
+    <t>Se ha comprobado que el dispositivo USB no autorizado es bloqueado.</t>
+  </si>
+  <si>
+    <t>Cuando se realiza un respaldo de las claves en el dispositivo USB, el sistema debe cifrar el respaldo usando una contraseña segura proporcionada por el usuario.</t>
+  </si>
+  <si>
+    <t>Respaldo de las claves criptográficas en el dispositivo USB</t>
+  </si>
+  <si>
+    <t>El sistema cifra el respaldo de las claves, asegurando que esté protegido contra accesos no autorizados</t>
+  </si>
+  <si>
+    <t>Se ha validado que el respaldo se cifra correctamente con una contraseña segura.</t>
+  </si>
+  <si>
+    <t>El sistema debe tener una disponibilidad del 95% del tiempo.</t>
+  </si>
+  <si>
+    <t>Fuente del Estímulo</t>
+  </si>
+  <si>
+    <t>Medida de la Respuesta</t>
+  </si>
+  <si>
+    <t>Durante un período de 30 días, la disponibilidad del sistema debe ser igual o superior al 95%.</t>
+  </si>
+  <si>
+    <t>Monitoreo de disponibilidad</t>
+  </si>
+  <si>
+    <t>Monitoreo continuo durante 30 días</t>
+  </si>
+  <si>
+    <t>El sistema mantiene una disponibilidad del 95% o superior durante el período evaluado.</t>
+  </si>
+  <si>
+    <t>La disponibilidad promedio del sistema es al menos del 95% durante el período de evaluación.</t>
+  </si>
+  <si>
+    <t>El sistema debe reportar cualquier caída en la disponibilidad que reduzca el tiempo operativo por debajo del 95%.</t>
+  </si>
+  <si>
+    <t>Sistema de monitoreo y reporte</t>
+  </si>
+  <si>
+    <t>Interrupción que afecta la disponibilidad</t>
+  </si>
+  <si>
+    <t>El sistema genera una alerta o informe cuando la disponibilidad cae por debajo del 95%.</t>
+  </si>
+  <si>
+    <t>El informe de disponibilidad muestra una caída y la notificación es enviada según el umbral establecido.</t>
+  </si>
+  <si>
+    <t>Se debe revisar mensualmente el informe de disponibilidad para asegurar que el sistema cumple con el 95% de disponibilidad.</t>
+  </si>
+  <si>
+    <t>Informes de disponibilidad</t>
+  </si>
+  <si>
+    <t>Revisión mensual de informes de disponibilidad</t>
+  </si>
+  <si>
+    <t>El informe mensual muestra que la disponibilidad del sistema cumple o supera el 95%.</t>
+  </si>
+  <si>
+    <t>El informe de disponibilidad mensual confirma que el sistema ha alcanzado al menos el 95% de disponibilidad.</t>
+  </si>
+  <si>
+    <t>En caso de fallo en un componente crítico, el sistema debe seguir funcionando sin afectar la disponibilidad total.</t>
+  </si>
+  <si>
+    <t>Simulación de fallos</t>
+  </si>
+  <si>
+    <t>Fallo en un componente crítico</t>
+  </si>
+  <si>
+    <t>Ambiente de prueba y simulación</t>
+  </si>
+  <si>
+    <t>El sistema sigue operativo y no se ve afectado en su totalidad.</t>
+  </si>
+  <si>
+    <t>El sistema mantiene la funcionalidad completa y la disponibilidad no se ve comprometida tras el fallo del componente.</t>
+  </si>
+  <si>
+    <t>Durante una prueba de resistencia, el sistema debe mostrar que las fallas parciales no impactan la disponibilidad general.</t>
+  </si>
+  <si>
+    <t>Pruebas de resistencia</t>
+  </si>
+  <si>
+    <t>Prueba de fallos parciales en el sistema</t>
+  </si>
+  <si>
+    <t>El sistema demuestra que puede manejar fallos parciales sin afectar la disponibilidad general.</t>
+  </si>
+  <si>
+    <t>El sistema maneja fallos parciales sin impactar la disponibilidad general durante las pruebas.</t>
+  </si>
+  <si>
+    <t>El sistema debe ser evaluado para asegurar que el diseño tolera fallos y proporciona alta disponibilidad durante situaciones de falla.</t>
+  </si>
+  <si>
+    <t>Evaluación de diseño</t>
+  </si>
+  <si>
+    <t>Evaluación del diseño para tolerancia a fallos</t>
+  </si>
+  <si>
+    <t>Ambiente de diseño y evaluación</t>
+  </si>
+  <si>
+    <t>El diseño del sistema muestra que está preparado para manejar fallos y mantener la disponibilidad.</t>
+  </si>
+  <si>
+    <t>El diseño cumple con los requisitos de tolerancia a fallos y mantiene la disponibilidad.</t>
+  </si>
+  <si>
+    <t>La aplicación debe ser compatible con diferentes sistemas operativos (Windows, macOS, Linux) para maximizar su alcance y adaptabilidad</t>
+  </si>
+  <si>
+    <t>La aplicación debe instalarse y ejecutarse correctamente en Windows, macOS y Linux.</t>
+  </si>
+  <si>
+    <t>Instalación y ejecución en Windows, macOS y Linux</t>
+  </si>
+  <si>
+    <t>Diferentes sistemas operativos</t>
+  </si>
+  <si>
+    <t>La aplicación se instala y ejecuta sin problemas en cada uno de los sistemas operativos.</t>
+  </si>
+  <si>
+    <t>La aplicación completa la instalación y ejecución en Windows, macOS y Linux sin errores.</t>
+  </si>
+  <si>
+    <t>La interfaz de usuario debe ajustarse automáticamente a diferentes resoluciones de pantalla en Windows, macOS y Linux.</t>
+  </si>
+  <si>
+    <t>Cambio de resolución en diferentes sistemas</t>
+  </si>
+  <si>
+    <t>Diferentes resoluciones de pantalla</t>
+  </si>
+  <si>
+    <t>La interfaz de usuario se ajusta adecuadamente en cada resolución de pantalla en todos los sistemas operativos.</t>
+  </si>
+  <si>
+    <t>La interfaz de usuario es consistente y funcional en todas las resoluciones de pantalla soportadas.</t>
+  </si>
+  <si>
+    <t>La aplicación debe poder instalarse desde un medio físico, como un CD o USB, en Windows, macOS y Linux.</t>
+  </si>
+  <si>
+    <t>Instalación desde CD o USB en diferentes sistemas</t>
+  </si>
+  <si>
+    <t>Instalación desde medio físico</t>
+  </si>
+  <si>
+    <t>La instalación desde CD o USB se completa correctamente en todos los sistemas operativos soportados.</t>
+  </si>
+  <si>
+    <t>La aplicación se instala correctamente desde un CD o USB en Windows, macOS y Linux.</t>
+  </si>
+  <si>
+    <t>La instalación de la aplicación no debe requerir la instalación de dependencias adicionales ni programas externos.</t>
+  </si>
+  <si>
+    <t>Instalación de la aplicación</t>
+  </si>
+  <si>
+    <t>Ambiente de prueba y despliegue</t>
+  </si>
+  <si>
+    <t>La aplicación se instala y ejecuta sin necesidad de programas o librerías adicionales.</t>
+  </si>
+  <si>
+    <t>La instalación se completa sin requerir dependencias adicionales o programas externos.</t>
+  </si>
+  <si>
+    <t>La aplicación debe proporcionar un instalador que incluya todas las dependencias necesarias para el funcionamiento.</t>
+  </si>
+  <si>
+    <t>Instalación usando el instalador incluido</t>
+  </si>
+  <si>
+    <t>El instalador incluye todas las librerías y dependencias necesarias, sin requerir instalación adicional.</t>
+  </si>
+  <si>
+    <t>La instalación se completa sin solicitar dependencias adicionales durante el proceso.</t>
+  </si>
+  <si>
+    <t>La documentación de instalación debe indicar claramente que no se requieren otros programas o librerías.</t>
+  </si>
+  <si>
+    <t>Consulta de la documentación de instalación</t>
+  </si>
+  <si>
+    <t>Ambiente de documentación</t>
+  </si>
+  <si>
+    <t>La documentación confirma que la aplicación no necesita otros programas o librerías para funcionar.</t>
+  </si>
+  <si>
+    <t>La documentación está clara y confirma la ausencia de requisitos adicionales.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Trade OFF/ Escenarios de calidad </t>
+  </si>
+  <si>
+    <t>El sistema debe de poder ejecutar la encriptación en menos de 30 segundos.</t>
+  </si>
+  <si>
+    <t>El sistema debe de poder ejecutar la desencriptación en menos de 30 segundos.</t>
+  </si>
+  <si>
+    <t>Cuando el sistema realice una operación de encriptación, debe completarla en menos de 30 segundos.</t>
+  </si>
+  <si>
+    <t>Ejecutar encriptación</t>
+  </si>
+  <si>
+    <t>La encriptación se completa en menos de 30 segundos.</t>
+  </si>
+  <si>
+    <t>Tiempo de encriptación medido desde el inicio hasta la finalización.</t>
+  </si>
+  <si>
+    <t>El sistema debe poder manejar múltiples solicitudes de encriptación simultáneamente sin que el tiempo de procesamiento para cada solicitud supere los 30 segundos.</t>
+  </si>
+  <si>
+    <t>Ejecutar encriptaciones concurrentes</t>
+  </si>
+  <si>
+    <t>Todas las solicitudes de encriptación se completan en menos de 30 segundos.</t>
+  </si>
+  <si>
+    <t>Tiempo de encriptación para cada solicitud medida individualmente.</t>
+  </si>
+  <si>
+    <t>Al realizar la encriptación de archivos grandes (por ejemplo, de 1 GB), el sistema debe completar la operación en menos de 30 segundos.</t>
+  </si>
+  <si>
+    <t>Ejecutar encriptación de archivos grandes</t>
+  </si>
+  <si>
+    <t>La encriptación de archivos de 1 GB se completa en menos de 30 segundos.</t>
+  </si>
+  <si>
+    <t>Cuando el sistema realice una operación de desencriptación, debe completarla en menos de 30 segundos.</t>
+  </si>
+  <si>
+    <t>Ejecutar desencriptación</t>
+  </si>
+  <si>
+    <t>La desencriptación se completa en menos de 30 segundos.</t>
+  </si>
+  <si>
+    <t>Tiempo de desencriptación medido desde el inicio hasta la finalización.</t>
+  </si>
+  <si>
+    <t>El sistema debe poder manejar múltiples solicitudes de desencriptación simultáneamente sin que el tiempo de procesamiento para cada solicitud supere los 30 segundos.</t>
+  </si>
+  <si>
+    <t>Ejecutar desencriptaciones concurrentes</t>
+  </si>
+  <si>
+    <t>Todas las solicitudes de desencriptación se completan en menos de 30 segundos.</t>
+  </si>
+  <si>
+    <t>Tiempo de desencriptación para cada solicitud medida individualmente.</t>
+  </si>
+  <si>
+    <t>Al realizar la desencriptación de archivos grandes (por ejemplo, de 1 GB), el sistema debe completar la operación en menos de 30 segundos.</t>
+  </si>
+  <si>
+    <t>Ejecutar desencriptación de archivos grandes</t>
+  </si>
+  <si>
+    <t>La desencriptación de archivos de 1 GB se completa en menos de 30 segundos.</t>
+  </si>
+  <si>
+    <t>Cuando se realice cualquier acción o evento importante en el sistema, se debe generar un registro detallado de la actividad.</t>
+  </si>
+  <si>
+    <t>Ejecutar acción o evento importante</t>
+  </si>
+  <si>
+    <t>Un registro detallado es generado y almacenado correctamente.</t>
+  </si>
+  <si>
+    <t>Existencia y detalle del registro de actividad.</t>
+  </si>
+  <si>
+    <t>Los registros de actividad deben ser accesibles para su revisión por personal autorizado sin necesidad de intervenciones adicionales.</t>
+  </si>
+  <si>
+    <t>Auditor</t>
+  </si>
+  <si>
+    <t>Acceder a registros de actividad</t>
+  </si>
+  <si>
+    <t>Los registros son accesibles y legibles sin problemas para personal autorizado.</t>
+  </si>
+  <si>
+    <t>Tiempo de acceso y calidad de la información disponible.</t>
+  </si>
+  <si>
+    <t>Los registros de actividad deben ser generados en tiempo real, sin retrasos significativos desde el evento que se registra.</t>
+  </si>
+  <si>
+    <t>Realizar una acción significativa</t>
+  </si>
+  <si>
+    <t>El registro es creado en tiempo real, inmediatamente después del evento.</t>
+  </si>
+  <si>
+    <t>Tiempo transcurrido desde el evento hasta la creación del registro.</t>
+  </si>
+  <si>
+    <t>El acceso a los registros de auditoría debe estar restringido a personal autorizado únicamente.</t>
+  </si>
+  <si>
+    <t>Intentar acceder a registros de auditoría sin autorización</t>
+  </si>
+  <si>
+    <t>El sistema restringe el acceso a personas no autorizadas.</t>
+  </si>
+  <si>
+    <t>Restricción de acceso y respuesta ante intentos no autorizados.</t>
+  </si>
+  <si>
+    <t>Los registros de auditoría deben ser accesibles únicamente a través de credenciales de acceso específicas para personal autorizado.</t>
+  </si>
+  <si>
+    <t>Acceder a registros de auditoría con credenciales válidas</t>
+  </si>
+  <si>
+    <t>El acceso a los registros es permitido solo con credenciales autorizadas.</t>
+  </si>
+  <si>
+    <t>Correcta autenticación y autorización para el acceso a registros.</t>
+  </si>
+  <si>
+    <t>Los registros de auditoría deben ser protegidos contra modificaciones no autorizadas.</t>
+  </si>
+  <si>
+    <t>Intentar modificar registros de auditoría</t>
+  </si>
+  <si>
+    <t>Los registros no se pueden modificar sin autorización adecuada.</t>
+  </si>
+  <si>
+    <t>Integridad y protección de los registros de auditoría.</t>
   </si>
 </sst>
 </file>
@@ -1153,7 +1759,7 @@
     <xf numFmtId="0" fontId="4" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="53">
+  <cellXfs count="56">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -1248,9 +1854,6 @@
     <xf numFmtId="10" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="0" xfId="3" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="7" fillId="10" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -1286,6 +1889,18 @@
     </xf>
     <xf numFmtId="0" fontId="6" fillId="11" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="3" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="4">
@@ -1379,7 +1994,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="es-MX"/>
+          <a:endParaRPr lang="es-CO"/>
         </a:p>
       </c:txPr>
     </c:title>
@@ -1858,7 +2473,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="es-MX"/>
+            <a:endParaRPr lang="es-CO"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="361250320"/>
@@ -1917,7 +2532,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="es-MX"/>
+            <a:endParaRPr lang="es-CO"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="361256080"/>
@@ -1959,7 +2574,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="es-MX"/>
+          <a:endParaRPr lang="es-CO"/>
         </a:p>
       </c:txPr>
     </c:legend>
@@ -1996,7 +2611,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="es-MX"/>
+      <a:endParaRPr lang="es-CO"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -2856,10 +3471,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F3"/>
+  <dimension ref="A1:F4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2868,28 +3483,33 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A1" s="9" t="s">
-        <v>0</v>
+      <c r="A1" t="s">
+        <v>375</v>
       </c>
       <c r="F1" s="1"/>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="9" t="s">
-        <v>15</v>
+        <v>0</v>
       </c>
       <c r="F2" s="1"/>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="F3" s="1"/>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4" s="9" t="s">
         <v>19</v>
       </c>
-      <c r="F3" s="1"/>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="A1" location="'Trade off '!A1" display="Trade off de QA" xr:uid="{DFE46B2E-658A-485B-9FB6-398B7CA63E1C}"/>
-    <hyperlink ref="A2" location="'Mapa Empatia'!A1" display="Mapa de Empatia " xr:uid="{E0A6560C-961F-4860-8ADD-F07043445D12}"/>
-    <hyperlink ref="A3" location="Caracterizacion!A1" display="Caractetizacion " xr:uid="{ED93357A-4E55-4391-83A1-412B54BBAC90}"/>
+    <hyperlink ref="A2" location="'Trade off '!A1" display="Trade off de QA" xr:uid="{DFE46B2E-658A-485B-9FB6-398B7CA63E1C}"/>
+    <hyperlink ref="A3" location="'Mapa Empatia'!A1" display="Mapa de Empatia " xr:uid="{E0A6560C-961F-4860-8ADD-F07043445D12}"/>
+    <hyperlink ref="A4" location="Caracterizacion!A1" display="Caractetizacion " xr:uid="{ED93357A-4E55-4391-83A1-412B54BBAC90}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -2897,7 +3517,7 @@
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9F952A68-CFD3-4455-8952-3067C8308151}">
-  <dimension ref="A1:I7"/>
+  <dimension ref="A1:I15"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -2969,9 +3589,125 @@
         <v>147</v>
       </c>
     </row>
+    <row r="12" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+      <c r="A12" s="54" t="s">
+        <v>112</v>
+      </c>
+      <c r="B12" s="54" t="s">
+        <v>113</v>
+      </c>
+      <c r="C12" s="54" t="s">
+        <v>311</v>
+      </c>
+      <c r="D12" s="54" t="s">
+        <v>115</v>
+      </c>
+      <c r="E12" s="54" t="s">
+        <v>116</v>
+      </c>
+      <c r="F12" s="54" t="s">
+        <v>117</v>
+      </c>
+      <c r="G12" s="54" t="s">
+        <v>118</v>
+      </c>
+      <c r="H12" s="54" t="s">
+        <v>312</v>
+      </c>
+      <c r="I12" s="54" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" ht="225" x14ac:dyDescent="0.25">
+      <c r="A13" s="10">
+        <v>1</v>
+      </c>
+      <c r="B13" s="10" t="s">
+        <v>328</v>
+      </c>
+      <c r="C13" s="10" t="s">
+        <v>329</v>
+      </c>
+      <c r="D13" s="10" t="s">
+        <v>330</v>
+      </c>
+      <c r="E13" s="10" t="s">
+        <v>124</v>
+      </c>
+      <c r="F13" s="10" t="s">
+        <v>331</v>
+      </c>
+      <c r="G13" s="10" t="s">
+        <v>332</v>
+      </c>
+      <c r="H13" s="10" t="s">
+        <v>333</v>
+      </c>
+      <c r="I13" s="10" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" ht="225" x14ac:dyDescent="0.25">
+      <c r="A14" s="10">
+        <v>2</v>
+      </c>
+      <c r="B14" s="10" t="s">
+        <v>334</v>
+      </c>
+      <c r="C14" s="10" t="s">
+        <v>335</v>
+      </c>
+      <c r="D14" s="10" t="s">
+        <v>336</v>
+      </c>
+      <c r="E14" s="10" t="s">
+        <v>124</v>
+      </c>
+      <c r="F14" s="10" t="s">
+        <v>331</v>
+      </c>
+      <c r="G14" s="10" t="s">
+        <v>337</v>
+      </c>
+      <c r="H14" s="10" t="s">
+        <v>338</v>
+      </c>
+      <c r="I14" s="10" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" ht="240" x14ac:dyDescent="0.25">
+      <c r="A15" s="10">
+        <v>3</v>
+      </c>
+      <c r="B15" s="10" t="s">
+        <v>339</v>
+      </c>
+      <c r="C15" s="10" t="s">
+        <v>340</v>
+      </c>
+      <c r="D15" s="10" t="s">
+        <v>341</v>
+      </c>
+      <c r="E15" s="10" t="s">
+        <v>124</v>
+      </c>
+      <c r="F15" s="10" t="s">
+        <v>342</v>
+      </c>
+      <c r="G15" s="10" t="s">
+        <v>343</v>
+      </c>
+      <c r="H15" s="10" t="s">
+        <v>344</v>
+      </c>
+      <c r="I15" s="10" t="s">
+        <v>128</v>
+      </c>
+    </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="A1" location="Caracterizacion!A1" display="Caracterizacion" xr:uid="{5954BB2F-9EED-4974-8B8A-32A3B81B5F94}"/>
+    <hyperlink ref="A1" location="Caracterizacion!A37" display="Caracterizacion" xr:uid="{5954BB2F-9EED-4974-8B8A-32A3B81B5F94}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -2980,7 +3716,7 @@
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E61622F7-0E97-45E4-AD8D-67A23570D199}">
-  <dimension ref="A1:I7"/>
+  <dimension ref="A1:I21"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -3050,6 +3786,195 @@
       </c>
       <c r="I7" t="s">
         <v>147</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A13" s="35" t="s">
+        <v>287</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A14" s="35" t="s">
+        <v>288</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A15" s="35" t="s">
+        <v>289</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+      <c r="A16" s="54" t="s">
+        <v>112</v>
+      </c>
+      <c r="B16" s="54" t="s">
+        <v>113</v>
+      </c>
+      <c r="C16" s="54" t="s">
+        <v>114</v>
+      </c>
+      <c r="D16" s="54" t="s">
+        <v>115</v>
+      </c>
+      <c r="E16" s="54" t="s">
+        <v>116</v>
+      </c>
+      <c r="F16" s="54" t="s">
+        <v>117</v>
+      </c>
+      <c r="G16" s="54" t="s">
+        <v>118</v>
+      </c>
+      <c r="H16" s="54" t="s">
+        <v>119</v>
+      </c>
+      <c r="I16" s="54" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" ht="210" x14ac:dyDescent="0.25">
+      <c r="A17" s="10">
+        <v>1</v>
+      </c>
+      <c r="B17" s="10" t="s">
+        <v>290</v>
+      </c>
+      <c r="C17" s="10" t="s">
+        <v>122</v>
+      </c>
+      <c r="D17" s="10" t="s">
+        <v>291</v>
+      </c>
+      <c r="E17" s="10" t="s">
+        <v>263</v>
+      </c>
+      <c r="F17" s="10" t="s">
+        <v>264</v>
+      </c>
+      <c r="G17" s="10" t="s">
+        <v>292</v>
+      </c>
+      <c r="H17" s="10" t="s">
+        <v>293</v>
+      </c>
+      <c r="I17" s="10" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" ht="225" x14ac:dyDescent="0.25">
+      <c r="A18" s="10">
+        <v>2</v>
+      </c>
+      <c r="B18" s="10" t="s">
+        <v>294</v>
+      </c>
+      <c r="C18" s="10" t="s">
+        <v>122</v>
+      </c>
+      <c r="D18" s="10" t="s">
+        <v>295</v>
+      </c>
+      <c r="E18" s="10" t="s">
+        <v>263</v>
+      </c>
+      <c r="F18" s="10" t="s">
+        <v>264</v>
+      </c>
+      <c r="G18" s="10" t="s">
+        <v>296</v>
+      </c>
+      <c r="H18" s="10" t="s">
+        <v>297</v>
+      </c>
+      <c r="I18" s="10" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" ht="225" x14ac:dyDescent="0.25">
+      <c r="A19" s="10">
+        <v>3</v>
+      </c>
+      <c r="B19" s="10" t="s">
+        <v>298</v>
+      </c>
+      <c r="C19" s="10" t="s">
+        <v>122</v>
+      </c>
+      <c r="D19" s="10" t="s">
+        <v>299</v>
+      </c>
+      <c r="E19" s="10" t="s">
+        <v>263</v>
+      </c>
+      <c r="F19" s="10" t="s">
+        <v>264</v>
+      </c>
+      <c r="G19" s="10" t="s">
+        <v>300</v>
+      </c>
+      <c r="H19" s="10" t="s">
+        <v>301</v>
+      </c>
+      <c r="I19" s="10" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" ht="180" x14ac:dyDescent="0.25">
+      <c r="A20" s="10">
+        <v>4</v>
+      </c>
+      <c r="B20" s="10" t="s">
+        <v>302</v>
+      </c>
+      <c r="C20" s="10" t="s">
+        <v>268</v>
+      </c>
+      <c r="D20" s="10" t="s">
+        <v>303</v>
+      </c>
+      <c r="E20" s="10" t="s">
+        <v>263</v>
+      </c>
+      <c r="F20" s="10" t="s">
+        <v>270</v>
+      </c>
+      <c r="G20" s="10" t="s">
+        <v>304</v>
+      </c>
+      <c r="H20" s="10" t="s">
+        <v>305</v>
+      </c>
+      <c r="I20" s="10" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" ht="240" x14ac:dyDescent="0.25">
+      <c r="A21" s="10">
+        <v>5</v>
+      </c>
+      <c r="B21" s="10" t="s">
+        <v>306</v>
+      </c>
+      <c r="C21" s="10" t="s">
+        <v>122</v>
+      </c>
+      <c r="D21" s="10" t="s">
+        <v>307</v>
+      </c>
+      <c r="E21" s="10" t="s">
+        <v>263</v>
+      </c>
+      <c r="F21" s="10" t="s">
+        <v>283</v>
+      </c>
+      <c r="G21" s="10" t="s">
+        <v>308</v>
+      </c>
+      <c r="H21" s="10" t="s">
+        <v>309</v>
+      </c>
+      <c r="I21" s="10" t="s">
+        <v>128</v>
       </c>
     </row>
   </sheetData>
@@ -3062,7 +3987,7 @@
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E889B929-B5B5-483A-BEEF-8B8890C6DDF7}">
-  <dimension ref="A1:I24"/>
+  <dimension ref="A1:I37"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -3143,74 +4068,74 @@
       <c r="A14" s="26" t="s">
         <v>104</v>
       </c>
-      <c r="B14" s="41" t="s">
+      <c r="B14" s="40" t="s">
         <v>105</v>
       </c>
-      <c r="C14" s="42"/>
-      <c r="D14" s="42"/>
-      <c r="E14" s="42"/>
-      <c r="F14" s="42"/>
-      <c r="G14" s="42"/>
-      <c r="H14" s="42"/>
-      <c r="I14" s="43"/>
+      <c r="C14" s="41"/>
+      <c r="D14" s="41"/>
+      <c r="E14" s="41"/>
+      <c r="F14" s="41"/>
+      <c r="G14" s="41"/>
+      <c r="H14" s="41"/>
+      <c r="I14" s="42"/>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A15" s="27" t="s">
         <v>106</v>
       </c>
-      <c r="B15" s="44" t="s">
+      <c r="B15" s="43" t="s">
         <v>107</v>
       </c>
-      <c r="C15" s="45"/>
-      <c r="D15" s="45"/>
-      <c r="E15" s="45"/>
-      <c r="F15" s="45"/>
-      <c r="G15" s="45"/>
-      <c r="H15" s="45"/>
-      <c r="I15" s="46"/>
+      <c r="C15" s="44"/>
+      <c r="D15" s="44"/>
+      <c r="E15" s="44"/>
+      <c r="F15" s="44"/>
+      <c r="G15" s="44"/>
+      <c r="H15" s="44"/>
+      <c r="I15" s="45"/>
     </row>
     <row r="16" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="27" t="s">
         <v>95</v>
       </c>
-      <c r="B16" s="47" t="s">
+      <c r="B16" s="46" t="s">
         <v>108</v>
       </c>
-      <c r="C16" s="48"/>
-      <c r="D16" s="48"/>
-      <c r="E16" s="48"/>
-      <c r="F16" s="48"/>
-      <c r="G16" s="48"/>
-      <c r="H16" s="48"/>
-      <c r="I16" s="49"/>
+      <c r="C16" s="47"/>
+      <c r="D16" s="47"/>
+      <c r="E16" s="47"/>
+      <c r="F16" s="47"/>
+      <c r="G16" s="47"/>
+      <c r="H16" s="47"/>
+      <c r="I16" s="48"/>
     </row>
     <row r="17" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="27" t="s">
         <v>109</v>
       </c>
-      <c r="B17" s="47" t="s">
+      <c r="B17" s="46" t="s">
         <v>110</v>
       </c>
-      <c r="C17" s="48"/>
-      <c r="D17" s="48"/>
-      <c r="E17" s="48"/>
-      <c r="F17" s="48"/>
-      <c r="G17" s="48"/>
-      <c r="H17" s="48"/>
-      <c r="I17" s="49"/>
+      <c r="C17" s="47"/>
+      <c r="D17" s="47"/>
+      <c r="E17" s="47"/>
+      <c r="F17" s="47"/>
+      <c r="G17" s="47"/>
+      <c r="H17" s="47"/>
+      <c r="I17" s="48"/>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A18" s="50" t="s">
+      <c r="A18" s="49" t="s">
         <v>111</v>
       </c>
-      <c r="B18" s="51"/>
-      <c r="C18" s="51"/>
-      <c r="D18" s="51"/>
-      <c r="E18" s="51"/>
-      <c r="F18" s="51"/>
-      <c r="G18" s="51"/>
-      <c r="H18" s="51"/>
-      <c r="I18" s="52"/>
+      <c r="B18" s="50"/>
+      <c r="C18" s="50"/>
+      <c r="D18" s="50"/>
+      <c r="E18" s="50"/>
+      <c r="F18" s="50"/>
+      <c r="G18" s="50"/>
+      <c r="H18" s="50"/>
+      <c r="I18" s="51"/>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A19" s="28" t="s">
@@ -3383,6 +4308,195 @@
         <v>144</v>
       </c>
       <c r="I24" s="34" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A29" s="35" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A30" s="35" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A31" s="35" t="s">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A32" s="54" t="s">
+        <v>112</v>
+      </c>
+      <c r="B32" s="54" t="s">
+        <v>113</v>
+      </c>
+      <c r="C32" s="54" t="s">
+        <v>114</v>
+      </c>
+      <c r="D32" s="54" t="s">
+        <v>115</v>
+      </c>
+      <c r="E32" s="54" t="s">
+        <v>116</v>
+      </c>
+      <c r="F32" s="54" t="s">
+        <v>117</v>
+      </c>
+      <c r="G32" s="54" t="s">
+        <v>118</v>
+      </c>
+      <c r="H32" s="54" t="s">
+        <v>119</v>
+      </c>
+      <c r="I32" s="54" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="33" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+      <c r="A33" s="10">
+        <v>1</v>
+      </c>
+      <c r="B33" s="10" t="s">
+        <v>261</v>
+      </c>
+      <c r="C33" s="10" t="s">
+        <v>122</v>
+      </c>
+      <c r="D33" s="10" t="s">
+        <v>262</v>
+      </c>
+      <c r="E33" s="10" t="s">
+        <v>263</v>
+      </c>
+      <c r="F33" s="10" t="s">
+        <v>264</v>
+      </c>
+      <c r="G33" s="10" t="s">
+        <v>265</v>
+      </c>
+      <c r="H33" s="10" t="s">
+        <v>266</v>
+      </c>
+      <c r="I33" s="10" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="34" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+      <c r="A34" s="10">
+        <v>2</v>
+      </c>
+      <c r="B34" s="10" t="s">
+        <v>267</v>
+      </c>
+      <c r="C34" s="10" t="s">
+        <v>268</v>
+      </c>
+      <c r="D34" s="10" t="s">
+        <v>269</v>
+      </c>
+      <c r="E34" s="10" t="s">
+        <v>263</v>
+      </c>
+      <c r="F34" s="10" t="s">
+        <v>270</v>
+      </c>
+      <c r="G34" s="10" t="s">
+        <v>271</v>
+      </c>
+      <c r="H34" s="10" t="s">
+        <v>272</v>
+      </c>
+      <c r="I34" s="10" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="35" spans="1:9" ht="60" x14ac:dyDescent="0.25">
+      <c r="A35" s="10">
+        <v>3</v>
+      </c>
+      <c r="B35" s="10" t="s">
+        <v>273</v>
+      </c>
+      <c r="C35" s="10" t="s">
+        <v>122</v>
+      </c>
+      <c r="D35" s="10" t="s">
+        <v>274</v>
+      </c>
+      <c r="E35" s="10" t="s">
+        <v>263</v>
+      </c>
+      <c r="F35" s="10" t="s">
+        <v>264</v>
+      </c>
+      <c r="G35" s="10" t="s">
+        <v>275</v>
+      </c>
+      <c r="H35" s="10" t="s">
+        <v>276</v>
+      </c>
+      <c r="I35" s="10" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="36" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+      <c r="A36" s="10">
+        <v>4</v>
+      </c>
+      <c r="B36" s="10" t="s">
+        <v>277</v>
+      </c>
+      <c r="C36" s="10" t="s">
+        <v>122</v>
+      </c>
+      <c r="D36" s="10" t="s">
+        <v>278</v>
+      </c>
+      <c r="E36" s="10" t="s">
+        <v>263</v>
+      </c>
+      <c r="F36" s="10" t="s">
+        <v>270</v>
+      </c>
+      <c r="G36" s="10" t="s">
+        <v>279</v>
+      </c>
+      <c r="H36" s="10" t="s">
+        <v>280</v>
+      </c>
+      <c r="I36" s="10" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="37" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+      <c r="A37" s="10">
+        <v>5</v>
+      </c>
+      <c r="B37" s="10" t="s">
+        <v>281</v>
+      </c>
+      <c r="C37" s="10" t="s">
+        <v>263</v>
+      </c>
+      <c r="D37" s="10" t="s">
+        <v>282</v>
+      </c>
+      <c r="E37" s="10" t="s">
+        <v>263</v>
+      </c>
+      <c r="F37" s="10" t="s">
+        <v>283</v>
+      </c>
+      <c r="G37" s="10" t="s">
+        <v>284</v>
+      </c>
+      <c r="H37" s="10" t="s">
+        <v>285</v>
+      </c>
+      <c r="I37" s="10" t="s">
         <v>128</v>
       </c>
     </row>
@@ -4066,10 +5180,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8A4C73B9-0AF9-4DE7-8A91-18F0737D3184}">
-  <dimension ref="A1:I152"/>
+  <dimension ref="A1:I156"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A116" workbookViewId="0">
-      <selection activeCell="E126" sqref="E126"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4112,6 +5226,9 @@
       <c r="C3" s="24" t="s">
         <v>90</v>
       </c>
+      <c r="D3" t="s">
+        <v>257</v>
+      </c>
       <c r="E3" s="10"/>
     </row>
     <row r="4" spans="1:9" ht="30" x14ac:dyDescent="0.25">
@@ -4123,6 +5240,9 @@
       </c>
       <c r="C4" s="24" t="s">
         <v>148</v>
+      </c>
+      <c r="D4" t="s">
+        <v>286</v>
       </c>
     </row>
     <row r="5" spans="1:9" ht="30" x14ac:dyDescent="0.25">
@@ -4321,7 +5441,7 @@
         <v>6</v>
       </c>
       <c r="B24" s="17" t="s">
-        <v>240</v>
+        <v>237</v>
       </c>
       <c r="E24" s="10"/>
     </row>
@@ -4329,7 +5449,7 @@
       <c r="A25" s="18" t="s">
         <v>6</v>
       </c>
-      <c r="B25" s="40" t="s">
+      <c r="B25" s="16" t="s">
         <v>164</v>
       </c>
     </row>
@@ -4337,7 +5457,7 @@
       <c r="A26" s="18" t="s">
         <v>6</v>
       </c>
-      <c r="B26" s="40" t="s">
+      <c r="B26" s="16" t="s">
         <v>165</v>
       </c>
       <c r="F26" s="11"/>
@@ -4346,7 +5466,7 @@
       <c r="A27" s="18" t="s">
         <v>6</v>
       </c>
-      <c r="B27" s="40" t="s">
+      <c r="B27" s="16" t="s">
         <v>166</v>
       </c>
       <c r="E27" s="10"/>
@@ -4356,7 +5476,7 @@
       <c r="A28" s="18" t="s">
         <v>6</v>
       </c>
-      <c r="B28" s="40" t="s">
+      <c r="B28" s="16" t="s">
         <v>162</v>
       </c>
       <c r="E28" s="10"/>
@@ -4366,7 +5486,7 @@
       <c r="A29" s="18" t="s">
         <v>6</v>
       </c>
-      <c r="B29" s="40" t="s">
+      <c r="B29" s="16" t="s">
         <v>163</v>
       </c>
       <c r="F29" s="11"/>
@@ -4375,11 +5495,8 @@
       <c r="A30" s="18" t="s">
         <v>6</v>
       </c>
-      <c r="B30" s="40" t="s">
+      <c r="B30" s="16" t="s">
         <v>167</v>
-      </c>
-      <c r="E30" s="40" t="s">
-        <v>169</v>
       </c>
       <c r="F30" s="11"/>
     </row>
@@ -4387,11 +5504,8 @@
       <c r="A31" s="18" t="s">
         <v>6</v>
       </c>
-      <c r="B31" s="40" t="s">
+      <c r="B31" s="16" t="s">
         <v>168</v>
-      </c>
-      <c r="E31" s="40" t="s">
-        <v>241</v>
       </c>
       <c r="F31" s="11"/>
     </row>
@@ -4399,110 +5513,123 @@
       <c r="A32" s="18" t="s">
         <v>6</v>
       </c>
-      <c r="B32" s="40" t="s">
+      <c r="B32" s="16" t="s">
         <v>170</v>
       </c>
-      <c r="E32" s="40" t="s">
+      <c r="C32" s="7" t="s">
+        <v>254</v>
+      </c>
+      <c r="E32" s="52"/>
+      <c r="F32" s="11"/>
+    </row>
+    <row r="33" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A33" s="18" t="s">
+        <v>6</v>
+      </c>
+      <c r="B33" s="16" t="s">
+        <v>169</v>
+      </c>
+      <c r="C33" s="7" t="s">
+        <v>255</v>
+      </c>
+      <c r="E33" s="53"/>
+      <c r="F33" s="11"/>
+    </row>
+    <row r="34" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A34" s="18" t="s">
+        <v>6</v>
+      </c>
+      <c r="B34" s="16" t="s">
+        <v>238</v>
+      </c>
+      <c r="C34" s="7" t="s">
+        <v>255</v>
+      </c>
+      <c r="E34" s="53"/>
+      <c r="F34" s="11"/>
+    </row>
+    <row r="35" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A35" s="18" t="s">
+        <v>6</v>
+      </c>
+      <c r="B35" s="16" t="s">
         <v>171</v>
       </c>
-      <c r="F32" s="11"/>
-    </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A33" s="19" t="s">
-        <v>2</v>
-      </c>
-      <c r="B33" s="36" t="s">
-        <v>160</v>
-      </c>
-      <c r="C33" s="24" t="s">
-        <v>149</v>
-      </c>
-      <c r="E33" s="10"/>
-      <c r="F33" s="11"/>
-    </row>
-    <row r="34" spans="1:6" ht="45" x14ac:dyDescent="0.25">
-      <c r="A34" s="19" t="s">
-        <v>2</v>
-      </c>
-      <c r="B34" s="15" t="s">
-        <v>59</v>
-      </c>
-      <c r="C34" s="24" t="s">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="35" spans="1:6" ht="45" x14ac:dyDescent="0.25">
-      <c r="A35" s="19" t="s">
-        <v>2</v>
-      </c>
-      <c r="B35" s="17" t="s">
-        <v>40</v>
-      </c>
+      <c r="C35" s="7" t="s">
+        <v>255</v>
+      </c>
+      <c r="E35" s="53"/>
       <c r="F35" s="11"/>
     </row>
-    <row r="36" spans="1:6" ht="45" x14ac:dyDescent="0.25">
-      <c r="A36" s="19" t="s">
-        <v>2</v>
-      </c>
-      <c r="B36" s="17" t="s">
-        <v>41</v>
-      </c>
-      <c r="E36" s="10"/>
+    <row r="36" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A36" s="18" t="s">
+        <v>6</v>
+      </c>
+      <c r="B36" s="16" t="s">
+        <v>256</v>
+      </c>
+      <c r="C36" s="7" t="s">
+        <v>255</v>
+      </c>
+      <c r="E36" s="53"/>
       <c r="F36" s="11"/>
     </row>
-    <row r="37" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A37" s="19" t="s">
         <v>2</v>
       </c>
-      <c r="B37" s="17" t="s">
-        <v>42</v>
-      </c>
+      <c r="B37" s="36" t="s">
+        <v>160</v>
+      </c>
+      <c r="C37" s="24" t="s">
+        <v>149</v>
+      </c>
+      <c r="D37" t="s">
+        <v>310</v>
+      </c>
+      <c r="E37" s="10"/>
       <c r="F37" s="11"/>
     </row>
     <row r="38" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A38" s="19" t="s">
         <v>2</v>
       </c>
-      <c r="B38" s="17" t="s">
-        <v>44</v>
-      </c>
-      <c r="C38" s="7" t="s">
-        <v>61</v>
-      </c>
-      <c r="E38" s="10"/>
-      <c r="F38" s="11"/>
+      <c r="B38" s="15" t="s">
+        <v>59</v>
+      </c>
+      <c r="C38" s="24" t="s">
+        <v>150</v>
+      </c>
+      <c r="D38" t="s">
+        <v>177</v>
+      </c>
     </row>
     <row r="39" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A39" s="19" t="s">
         <v>2</v>
       </c>
       <c r="B39" s="17" t="s">
-        <v>43</v>
-      </c>
-      <c r="E39" s="10"/>
+        <v>40</v>
+      </c>
       <c r="F39" s="11"/>
     </row>
-    <row r="40" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A40" s="19" t="s">
         <v>2</v>
       </c>
       <c r="B40" s="17" t="s">
-        <v>63</v>
+        <v>41</v>
       </c>
       <c r="E40" s="10"/>
       <c r="F40" s="11"/>
     </row>
-    <row r="41" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A41" s="19" t="s">
         <v>2</v>
       </c>
       <c r="B41" s="17" t="s">
-        <v>64</v>
-      </c>
-      <c r="C41" s="7" t="s">
-        <v>62</v>
-      </c>
-      <c r="E41" s="10"/>
+        <v>42</v>
+      </c>
       <c r="F41" s="11"/>
     </row>
     <row r="42" spans="1:6" ht="45" x14ac:dyDescent="0.25">
@@ -4510,16 +5637,20 @@
         <v>2</v>
       </c>
       <c r="B42" s="17" t="s">
-        <v>45</v>
-      </c>
+        <v>44</v>
+      </c>
+      <c r="C42" s="7" t="s">
+        <v>61</v>
+      </c>
+      <c r="E42" s="10"/>
       <c r="F42" s="11"/>
     </row>
-    <row r="43" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A43" s="19" t="s">
         <v>2</v>
       </c>
-      <c r="B43" s="16" t="s">
-        <v>242</v>
+      <c r="B43" s="17" t="s">
+        <v>43</v>
       </c>
       <c r="E43" s="10"/>
       <c r="F43" s="11"/>
@@ -4528,8 +5659,8 @@
       <c r="A44" s="19" t="s">
         <v>2</v>
       </c>
-      <c r="B44" s="16" t="s">
-        <v>172</v>
+      <c r="B44" s="17" t="s">
+        <v>63</v>
       </c>
       <c r="E44" s="10"/>
       <c r="F44" s="11"/>
@@ -4538,8 +5669,11 @@
       <c r="A45" s="19" t="s">
         <v>2</v>
       </c>
-      <c r="B45" s="16" t="s">
-        <v>173</v>
+      <c r="B45" s="17" t="s">
+        <v>64</v>
+      </c>
+      <c r="C45" s="7" t="s">
+        <v>62</v>
       </c>
       <c r="E45" s="10"/>
       <c r="F45" s="11"/>
@@ -4548,18 +5682,17 @@
       <c r="A46" s="19" t="s">
         <v>2</v>
       </c>
-      <c r="B46" s="40" t="s">
-        <v>174</v>
-      </c>
-      <c r="E46" s="10"/>
+      <c r="B46" s="17" t="s">
+        <v>45</v>
+      </c>
       <c r="F46" s="11"/>
     </row>
     <row r="47" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A47" s="19" t="s">
         <v>2</v>
       </c>
-      <c r="B47" s="40" t="s">
-        <v>175</v>
+      <c r="B47" s="16" t="s">
+        <v>239</v>
       </c>
       <c r="E47" s="10"/>
       <c r="F47" s="11"/>
@@ -4568,187 +5701,192 @@
       <c r="A48" s="19" t="s">
         <v>2</v>
       </c>
-      <c r="B48" s="40" t="s">
-        <v>176</v>
-      </c>
-    </row>
-    <row r="49" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+      <c r="B48" s="16" t="s">
+        <v>172</v>
+      </c>
+      <c r="E48" s="10"/>
+      <c r="F48" s="11"/>
+    </row>
+    <row r="49" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A49" s="19" t="s">
         <v>2</v>
       </c>
-      <c r="B49" s="40" t="s">
-        <v>177</v>
+      <c r="B49" s="16" t="s">
+        <v>173</v>
       </c>
       <c r="E49" s="10"/>
-    </row>
-    <row r="50" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="F49" s="11"/>
+    </row>
+    <row r="50" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A50" s="19" t="s">
         <v>2</v>
       </c>
-      <c r="B50" s="40" t="s">
-        <v>178</v>
+      <c r="B50" s="16" t="s">
+        <v>174</v>
       </c>
       <c r="E50" s="10"/>
-    </row>
-    <row r="51" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F50" s="11"/>
+    </row>
+    <row r="51" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A51" s="19" t="s">
         <v>2</v>
       </c>
-      <c r="B51" s="22"/>
-    </row>
-    <row r="52" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B51" s="16" t="s">
+        <v>175</v>
+      </c>
+      <c r="E51" s="10"/>
+      <c r="F51" s="11"/>
+    </row>
+    <row r="52" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A52" s="19" t="s">
         <v>2</v>
       </c>
-      <c r="B52" s="22"/>
-      <c r="E52" s="10"/>
-    </row>
-    <row r="53" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B52" s="16" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="53" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A53" s="19" t="s">
         <v>2</v>
       </c>
-      <c r="B53" s="22"/>
+      <c r="B53" s="16" t="s">
+        <v>177</v>
+      </c>
       <c r="E53" s="10"/>
     </row>
-    <row r="54" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A54" s="19" t="s">
         <v>2</v>
       </c>
-      <c r="B54" s="22"/>
+      <c r="B54" s="16" t="s">
+        <v>178</v>
+      </c>
       <c r="E54" s="10"/>
     </row>
-    <row r="55" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A55" s="19" t="s">
         <v>2</v>
       </c>
       <c r="B55" s="22"/>
-      <c r="E55" s="10"/>
-    </row>
-    <row r="56" spans="1:5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="56" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A56" s="19" t="s">
         <v>2</v>
       </c>
       <c r="B56" s="22"/>
       <c r="E56" s="10"/>
     </row>
-    <row r="57" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A57" s="19" t="s">
         <v>2</v>
       </c>
       <c r="B57" s="22"/>
       <c r="E57" s="10"/>
     </row>
-    <row r="58" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A58" s="19" t="s">
         <v>2</v>
       </c>
       <c r="B58" s="22"/>
       <c r="E58" s="10"/>
     </row>
-    <row r="59" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A59" s="19" t="s">
         <v>2</v>
       </c>
       <c r="B59" s="22"/>
       <c r="E59" s="10"/>
     </row>
-    <row r="60" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A60" s="19" t="s">
         <v>2</v>
       </c>
       <c r="B60" s="22"/>
       <c r="E60" s="10"/>
     </row>
-    <row r="61" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A61" s="19" t="s">
         <v>2</v>
       </c>
       <c r="B61" s="22"/>
       <c r="E61" s="10"/>
     </row>
-    <row r="62" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A62" s="19" t="s">
         <v>2</v>
       </c>
       <c r="B62" s="22"/>
-    </row>
-    <row r="63" spans="1:5" ht="45" x14ac:dyDescent="0.25">
-      <c r="A63" s="20" t="s">
-        <v>8</v>
-      </c>
-      <c r="B63" s="15" t="s">
-        <v>46</v>
-      </c>
-      <c r="C63" s="24" t="s">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="64" spans="1:5" ht="45" x14ac:dyDescent="0.25">
-      <c r="A64" s="20" t="s">
-        <v>8</v>
-      </c>
-      <c r="B64" s="15" t="s">
-        <v>47</v>
-      </c>
-      <c r="C64" s="24" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="65" spans="1:5" ht="45" x14ac:dyDescent="0.25">
-      <c r="A65" s="20" t="s">
-        <v>8</v>
-      </c>
-      <c r="B65" s="15" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="66" spans="1:5" ht="45" x14ac:dyDescent="0.25">
-      <c r="A66" s="20" t="s">
-        <v>8</v>
-      </c>
-      <c r="B66" s="16" t="s">
-        <v>49</v>
-      </c>
-      <c r="E66" s="10"/>
+      <c r="E62" s="10"/>
+    </row>
+    <row r="63" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A63" s="19" t="s">
+        <v>2</v>
+      </c>
+      <c r="B63" s="22"/>
+      <c r="E63" s="10"/>
+    </row>
+    <row r="64" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A64" s="19" t="s">
+        <v>2</v>
+      </c>
+      <c r="B64" s="22"/>
+      <c r="E64" s="10"/>
+    </row>
+    <row r="65" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A65" s="19" t="s">
+        <v>2</v>
+      </c>
+      <c r="B65" s="22"/>
+      <c r="E65" s="10"/>
+    </row>
+    <row r="66" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A66" s="19" t="s">
+        <v>2</v>
+      </c>
+      <c r="B66" s="22"/>
     </row>
     <row r="67" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A67" s="20" t="s">
         <v>8</v>
       </c>
-      <c r="B67" s="16" t="s">
-        <v>50</v>
-      </c>
-      <c r="E67" s="10"/>
+      <c r="B67" s="15" t="s">
+        <v>46</v>
+      </c>
+      <c r="C67" s="24" t="s">
+        <v>151</v>
+      </c>
+      <c r="D67" t="s">
+        <v>345</v>
+      </c>
     </row>
     <row r="68" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A68" s="20" t="s">
         <v>8</v>
       </c>
-      <c r="B68" s="16" t="s">
-        <v>51</v>
-      </c>
-      <c r="C68" s="7" t="s">
-        <v>65</v>
-      </c>
-      <c r="E68" s="10"/>
-    </row>
-    <row r="69" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="B68" s="15" t="s">
+        <v>47</v>
+      </c>
+      <c r="C68" s="24" t="s">
+        <v>152</v>
+      </c>
+      <c r="D68" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="69" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A69" s="20" t="s">
         <v>8</v>
       </c>
-      <c r="B69" s="16" t="s">
-        <v>52</v>
-      </c>
-      <c r="C69" s="7" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="70" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B69" s="15" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="70" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A70" s="20" t="s">
         <v>8</v>
       </c>
-      <c r="B70" s="17" t="s">
-        <v>88</v>
+      <c r="B70" s="16" t="s">
+        <v>49</v>
       </c>
       <c r="E70" s="10"/>
     </row>
@@ -4756,118 +5894,138 @@
       <c r="A71" s="20" t="s">
         <v>8</v>
       </c>
-      <c r="B71" s="40" t="s">
-        <v>181</v>
-      </c>
-    </row>
-    <row r="72" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="B71" s="16" t="s">
+        <v>50</v>
+      </c>
+      <c r="E71" s="10"/>
+    </row>
+    <row r="72" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A72" s="20" t="s">
         <v>8</v>
       </c>
-      <c r="B72" s="40" t="s">
-        <v>179</v>
+      <c r="B72" s="16" t="s">
+        <v>51</v>
+      </c>
+      <c r="C72" s="7" t="s">
+        <v>65</v>
       </c>
       <c r="E72" s="10"/>
     </row>
-    <row r="73" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A73" s="20" t="s">
         <v>8</v>
       </c>
-      <c r="B73" s="40" t="s">
-        <v>180</v>
-      </c>
-      <c r="E73" s="10" t="s">
-        <v>182</v>
-      </c>
-    </row>
-    <row r="74" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="B73" s="16" t="s">
+        <v>52</v>
+      </c>
+      <c r="C73" s="7" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="74" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A74" s="20" t="s">
         <v>8</v>
       </c>
-      <c r="B74" s="40" t="s">
-        <v>243</v>
-      </c>
-      <c r="E74" s="10" t="s">
-        <v>183</v>
-      </c>
-    </row>
-    <row r="75" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="B74" s="17" t="s">
+        <v>88</v>
+      </c>
+      <c r="E74" s="10"/>
+    </row>
+    <row r="75" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A75" s="20" t="s">
         <v>8</v>
       </c>
-      <c r="B75" s="17" t="s">
-        <v>244</v>
-      </c>
-      <c r="E75" s="10"/>
+      <c r="B75" s="16" t="s">
+        <v>181</v>
+      </c>
     </row>
     <row r="76" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A76" s="20" t="s">
         <v>8</v>
       </c>
-      <c r="B76" s="10" t="s">
-        <v>245</v>
-      </c>
-      <c r="E76" s="10" t="s">
-        <v>184</v>
-      </c>
-    </row>
-    <row r="77" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+      <c r="B76" s="16" t="s">
+        <v>179</v>
+      </c>
+      <c r="E76" s="10"/>
+    </row>
+    <row r="77" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A77" s="20" t="s">
         <v>8</v>
       </c>
-      <c r="B77" s="10" t="s">
-        <v>187</v>
-      </c>
-      <c r="E77" s="10"/>
+      <c r="B77" s="16" t="s">
+        <v>180</v>
+      </c>
     </row>
     <row r="78" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A78" s="20" t="s">
         <v>8</v>
       </c>
-      <c r="B78" s="22"/>
+      <c r="B78" s="16" t="s">
+        <v>240</v>
+      </c>
       <c r="E78" s="10" t="s">
-        <v>185</v>
-      </c>
-    </row>
-    <row r="79" spans="1:5" x14ac:dyDescent="0.25">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="79" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A79" s="20" t="s">
         <v>8</v>
       </c>
-      <c r="B79" s="22"/>
+      <c r="B79" s="17" t="s">
+        <v>241</v>
+      </c>
       <c r="E79" s="10"/>
     </row>
-    <row r="80" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A80" s="20" t="s">
         <v>8</v>
       </c>
-      <c r="B80" s="22"/>
-      <c r="E80" s="10"/>
-    </row>
-    <row r="81" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B80" s="17" t="s">
+        <v>242</v>
+      </c>
+      <c r="E80" s="10" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="81" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A81" s="20" t="s">
         <v>8</v>
       </c>
-      <c r="B81" s="22"/>
+      <c r="B81" s="17" t="s">
+        <v>187</v>
+      </c>
       <c r="E81" s="10"/>
     </row>
-    <row r="82" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A82" s="20" t="s">
         <v>8</v>
       </c>
-      <c r="B82" s="22"/>
-    </row>
-    <row r="83" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B82" s="17" t="s">
+        <v>182</v>
+      </c>
+      <c r="C82" s="7" t="s">
+        <v>244</v>
+      </c>
+      <c r="E82" s="10" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="83" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A83" s="20" t="s">
         <v>8</v>
       </c>
-      <c r="B83" s="22"/>
+      <c r="B83" s="17" t="s">
+        <v>186</v>
+      </c>
       <c r="E83" s="10"/>
     </row>
     <row r="84" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A84" s="20" t="s">
         <v>8</v>
       </c>
-      <c r="B84" s="22"/>
+      <c r="B84" s="17" t="s">
+        <v>250</v>
+      </c>
       <c r="E84" s="10"/>
     </row>
     <row r="85" spans="1:5" x14ac:dyDescent="0.25">
@@ -4877,14 +6035,11 @@
       <c r="B85" s="22"/>
       <c r="E85" s="10"/>
     </row>
-    <row r="86" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A86" s="20" t="s">
         <v>8</v>
       </c>
       <c r="B86" s="22"/>
-      <c r="E86" s="10" t="s">
-        <v>186</v>
-      </c>
     </row>
     <row r="87" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A87" s="20" t="s">
@@ -4898,6 +6053,7 @@
         <v>8</v>
       </c>
       <c r="B88" s="22"/>
+      <c r="E88" s="10"/>
     </row>
     <row r="89" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A89" s="20" t="s">
@@ -4911,7 +6067,6 @@
         <v>8</v>
       </c>
       <c r="B90" s="22"/>
-      <c r="E90" s="10"/>
     </row>
     <row r="91" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A91" s="20" t="s">
@@ -4925,221 +6080,227 @@
         <v>8</v>
       </c>
       <c r="B92" s="22"/>
-      <c r="E92" s="10"/>
-    </row>
-    <row r="93" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A93" s="21" t="s">
-        <v>14</v>
-      </c>
-      <c r="B93" s="14" t="s">
-        <v>32</v>
-      </c>
-      <c r="C93" s="24" t="s">
-        <v>153</v>
-      </c>
+    </row>
+    <row r="93" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A93" s="20" t="s">
+        <v>8</v>
+      </c>
+      <c r="B93" s="22"/>
       <c r="E93" s="10"/>
     </row>
-    <row r="94" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A94" s="21" t="s">
-        <v>14</v>
-      </c>
-      <c r="B94" s="14" t="s">
-        <v>30</v>
-      </c>
-      <c r="C94" s="24" t="s">
-        <v>154</v>
-      </c>
+    <row r="94" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A94" s="20" t="s">
+        <v>8</v>
+      </c>
+      <c r="B94" s="22"/>
       <c r="E94" s="10"/>
     </row>
-    <row r="95" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A95" s="21" t="s">
-        <v>14</v>
-      </c>
-      <c r="B95" s="14" t="s">
-        <v>31</v>
-      </c>
+    <row r="95" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A95" s="20" t="s">
+        <v>8</v>
+      </c>
+      <c r="B95" s="22"/>
       <c r="E95" s="10"/>
     </row>
-    <row r="96" spans="1:5" ht="45" x14ac:dyDescent="0.25">
-      <c r="A96" s="21" t="s">
-        <v>14</v>
-      </c>
-      <c r="B96" s="16" t="s">
-        <v>54</v>
-      </c>
-      <c r="E96" s="10" t="s">
-        <v>188</v>
-      </c>
-    </row>
-    <row r="97" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A96" s="20" t="s">
+        <v>8</v>
+      </c>
+      <c r="B96" s="22"/>
+      <c r="E96" s="10"/>
+    </row>
+    <row r="97" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A97" s="21" t="s">
         <v>14</v>
       </c>
-      <c r="B97" s="16" t="s">
-        <v>55</v>
-      </c>
-      <c r="E97" s="40" t="s">
-        <v>189</v>
-      </c>
-    </row>
-    <row r="98" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+      <c r="B97" s="14" t="s">
+        <v>32</v>
+      </c>
+      <c r="C97" s="24" t="s">
+        <v>153</v>
+      </c>
+      <c r="D97" s="35" t="s">
+        <v>376</v>
+      </c>
+      <c r="E97" s="10"/>
+    </row>
+    <row r="98" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A98" s="21" t="s">
         <v>14</v>
       </c>
-      <c r="B98" s="16" t="s">
-        <v>56</v>
-      </c>
-      <c r="E98" s="10" t="s">
-        <v>190</v>
-      </c>
-    </row>
-    <row r="99" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+      <c r="B98" s="14" t="s">
+        <v>30</v>
+      </c>
+      <c r="C98" s="24" t="s">
+        <v>154</v>
+      </c>
+      <c r="D98" s="35" t="s">
+        <v>377</v>
+      </c>
+      <c r="E98" s="10"/>
+    </row>
+    <row r="99" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A99" s="21" t="s">
         <v>14</v>
       </c>
-      <c r="B99" s="16" t="s">
-        <v>53</v>
-      </c>
-      <c r="E99" s="10" t="s">
-        <v>191</v>
-      </c>
-    </row>
-    <row r="100" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B99" s="14" t="s">
+        <v>31</v>
+      </c>
+      <c r="E99" s="10"/>
+    </row>
+    <row r="100" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A100" s="21" t="s">
         <v>14</v>
       </c>
-      <c r="B100" s="22" t="s">
-        <v>86</v>
-      </c>
-      <c r="E100" s="10"/>
-    </row>
-    <row r="101" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="B100" s="16" t="s">
+        <v>54</v>
+      </c>
+      <c r="E100" s="10" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="101" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A101" s="21" t="s">
         <v>14</v>
       </c>
-      <c r="B101" s="22" t="s">
-        <v>87</v>
-      </c>
-      <c r="E101" s="10"/>
-    </row>
-    <row r="102" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="B101" s="16" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="102" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A102" s="21" t="s">
         <v>14</v>
       </c>
-      <c r="B102" s="10" t="s">
-        <v>193</v>
-      </c>
-      <c r="E102" s="10"/>
-    </row>
-    <row r="103" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="B102" s="16" t="s">
+        <v>56</v>
+      </c>
+      <c r="E102" s="10" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="103" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A103" s="21" t="s">
         <v>14</v>
       </c>
-      <c r="B103" s="10" t="s">
-        <v>246</v>
-      </c>
-      <c r="E103" s="10"/>
-    </row>
-    <row r="104" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="B103" s="16" t="s">
+        <v>53</v>
+      </c>
+      <c r="E103" s="10" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="104" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A104" s="21" t="s">
         <v>14</v>
       </c>
-      <c r="B104" s="22"/>
-      <c r="E104" s="10" t="s">
-        <v>192</v>
-      </c>
-    </row>
-    <row r="105" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B104" s="16" t="s">
+        <v>86</v>
+      </c>
+      <c r="E104" s="10"/>
+    </row>
+    <row r="105" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A105" s="21" t="s">
         <v>14</v>
       </c>
-      <c r="B105" s="22"/>
-    </row>
-    <row r="106" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B105" s="16" t="s">
+        <v>87</v>
+      </c>
+      <c r="E105" s="10"/>
+    </row>
+    <row r="106" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A106" s="21" t="s">
         <v>14</v>
       </c>
-      <c r="B106" s="22"/>
-      <c r="E106" s="10" t="s">
-        <v>194</v>
-      </c>
+      <c r="B106" s="16" t="s">
+        <v>193</v>
+      </c>
+      <c r="E106" s="10"/>
     </row>
     <row r="107" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A107" s="21" t="s">
         <v>14</v>
       </c>
-      <c r="B107" s="22"/>
-      <c r="E107" s="10" t="s">
-        <v>195</v>
-      </c>
-    </row>
-    <row r="108" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B107" s="16" t="s">
+        <v>243</v>
+      </c>
+      <c r="E107" s="10"/>
+    </row>
+    <row r="108" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A108" s="21" t="s">
         <v>14</v>
       </c>
-      <c r="B108" s="22"/>
-    </row>
-    <row r="109" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="B108" s="16" t="s">
+        <v>189</v>
+      </c>
+      <c r="E108" s="10" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="109" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A109" s="21" t="s">
         <v>14</v>
       </c>
-      <c r="B109" s="22"/>
-      <c r="E109" s="10" t="s">
-        <v>196</v>
-      </c>
-    </row>
-    <row r="110" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B109" s="16" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="110" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A110" s="21" t="s">
         <v>14</v>
       </c>
-      <c r="B110" s="22"/>
+      <c r="B110" s="16" t="s">
+        <v>247</v>
+      </c>
       <c r="E110" s="10" t="s">
-        <v>197</v>
-      </c>
-    </row>
-    <row r="111" spans="1:5" x14ac:dyDescent="0.25">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="111" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A111" s="21" t="s">
         <v>14</v>
       </c>
-      <c r="B111" s="22"/>
+      <c r="B111" s="16" t="s">
+        <v>248</v>
+      </c>
       <c r="E111" s="10" t="s">
-        <v>198</v>
-      </c>
-    </row>
-    <row r="112" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="112" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A112" s="21" t="s">
         <v>14</v>
       </c>
-      <c r="B112" s="22"/>
-      <c r="E112" s="10" t="s">
-        <v>199</v>
+      <c r="B112" s="16" t="s">
+        <v>251</v>
       </c>
     </row>
     <row r="113" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A113" s="21" t="s">
         <v>14</v>
       </c>
-      <c r="B113" s="22"/>
+      <c r="B113" s="16" t="s">
+        <v>252</v>
+      </c>
       <c r="E113" s="10" t="s">
-        <v>200</v>
-      </c>
-    </row>
-    <row r="114" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="114" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A114" s="21" t="s">
         <v>14</v>
       </c>
       <c r="B114" s="22"/>
       <c r="E114" s="10" t="s">
-        <v>201</v>
-      </c>
-    </row>
-    <row r="115" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="115" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A115" s="21" t="s">
         <v>14</v>
       </c>
       <c r="B115" s="22"/>
       <c r="E115" s="10" t="s">
-        <v>202</v>
+        <v>198</v>
       </c>
     </row>
     <row r="116" spans="1:5" ht="30" x14ac:dyDescent="0.25">
@@ -5148,7 +6309,7 @@
       </c>
       <c r="B116" s="22"/>
       <c r="E116" s="10" t="s">
-        <v>203</v>
+        <v>199</v>
       </c>
     </row>
     <row r="117" spans="1:5" ht="30" x14ac:dyDescent="0.25">
@@ -5157,25 +6318,25 @@
       </c>
       <c r="B117" s="22"/>
       <c r="E117" s="10" t="s">
-        <v>204</v>
-      </c>
-    </row>
-    <row r="118" spans="1:5" x14ac:dyDescent="0.25">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="118" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A118" s="21" t="s">
         <v>14</v>
       </c>
       <c r="B118" s="22"/>
       <c r="E118" s="10" t="s">
-        <v>205</v>
-      </c>
-    </row>
-    <row r="119" spans="1:5" x14ac:dyDescent="0.25">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="119" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A119" s="21" t="s">
         <v>14</v>
       </c>
       <c r="B119" s="22"/>
       <c r="E119" s="10" t="s">
-        <v>206</v>
+        <v>202</v>
       </c>
     </row>
     <row r="120" spans="1:5" ht="30" x14ac:dyDescent="0.25">
@@ -5184,72 +6345,61 @@
       </c>
       <c r="B120" s="22"/>
       <c r="E120" s="10" t="s">
-        <v>207</v>
-      </c>
-    </row>
-    <row r="121" spans="1:5" x14ac:dyDescent="0.25">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="121" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A121" s="21" t="s">
         <v>14</v>
       </c>
       <c r="B121" s="22"/>
       <c r="E121" s="10" t="s">
-        <v>208</v>
-      </c>
-    </row>
-    <row r="122" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="122" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A122" s="21" t="s">
         <v>14</v>
       </c>
       <c r="B122" s="22"/>
       <c r="E122" s="10" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="123" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A123" s="21" t="s">
+        <v>14</v>
+      </c>
+      <c r="B123" s="22"/>
+      <c r="E123" s="10" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="124" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A124" s="21" t="s">
+        <v>14</v>
+      </c>
+      <c r="B124" s="22"/>
+      <c r="E124" s="10" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="125" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A125" s="21" t="s">
+        <v>14</v>
+      </c>
+      <c r="B125" s="22"/>
+      <c r="E125" s="10" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="126" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A126" s="21" t="s">
+        <v>14</v>
+      </c>
+      <c r="B126" s="22"/>
+      <c r="E126" s="10" t="s">
         <v>209</v>
-      </c>
-    </row>
-    <row r="123" spans="1:5" ht="45" x14ac:dyDescent="0.25">
-      <c r="A123" s="23" t="s">
-        <v>12</v>
-      </c>
-      <c r="B123" s="15" t="s">
-        <v>67</v>
-      </c>
-      <c r="C123" s="24" t="s">
-        <v>155</v>
-      </c>
-    </row>
-    <row r="124" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A124" s="23" t="s">
-        <v>12</v>
-      </c>
-      <c r="B124" s="15" t="s">
-        <v>68</v>
-      </c>
-      <c r="C124" s="24" t="s">
-        <v>156</v>
-      </c>
-      <c r="E124" s="10" t="s">
-        <v>211</v>
-      </c>
-    </row>
-    <row r="125" spans="1:5" ht="45" x14ac:dyDescent="0.25">
-      <c r="A125" s="23" t="s">
-        <v>12</v>
-      </c>
-      <c r="B125" s="15" t="s">
-        <v>69</v>
-      </c>
-      <c r="E125" s="10" t="s">
-        <v>212</v>
-      </c>
-    </row>
-    <row r="126" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A126" s="23" t="s">
-        <v>12</v>
-      </c>
-      <c r="B126" s="15" t="s">
-        <v>70</v>
-      </c>
-      <c r="E126" s="10" t="s">
-        <v>213</v>
       </c>
     </row>
     <row r="127" spans="1:5" ht="45" x14ac:dyDescent="0.25">
@@ -5257,10 +6407,13 @@
         <v>12</v>
       </c>
       <c r="B127" s="15" t="s">
-        <v>72</v>
-      </c>
-      <c r="E127" s="10" t="s">
-        <v>214</v>
+        <v>67</v>
+      </c>
+      <c r="C127" s="24" t="s">
+        <v>155</v>
+      </c>
+      <c r="D127" t="s">
+        <v>67</v>
       </c>
     </row>
     <row r="128" spans="1:5" ht="30" x14ac:dyDescent="0.25">
@@ -5268,32 +6421,34 @@
         <v>12</v>
       </c>
       <c r="B128" s="15" t="s">
-        <v>74</v>
-      </c>
-      <c r="E128" s="10" t="s">
-        <v>215</v>
-      </c>
+        <v>68</v>
+      </c>
+      <c r="C128" s="24" t="s">
+        <v>156</v>
+      </c>
+      <c r="D128" t="s">
+        <v>72</v>
+      </c>
+      <c r="E128" s="10"/>
     </row>
     <row r="129" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A129" s="23" t="s">
         <v>12</v>
       </c>
       <c r="B129" s="15" t="s">
-        <v>75</v>
-      </c>
-      <c r="E129" s="10" t="s">
-        <v>216</v>
-      </c>
+        <v>69</v>
+      </c>
+      <c r="E129" s="10"/>
     </row>
     <row r="130" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A130" s="23" t="s">
         <v>12</v>
       </c>
       <c r="B130" s="15" t="s">
-        <v>76</v>
+        <v>70</v>
       </c>
       <c r="E130" s="10" t="s">
-        <v>217</v>
+        <v>211</v>
       </c>
     </row>
     <row r="131" spans="1:5" ht="45" x14ac:dyDescent="0.25">
@@ -5301,79 +6456,73 @@
         <v>12</v>
       </c>
       <c r="B131" s="15" t="s">
-        <v>78</v>
+        <v>72</v>
       </c>
       <c r="E131" s="10" t="s">
-        <v>218</v>
-      </c>
-    </row>
-    <row r="132" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="132" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A132" s="23" t="s">
         <v>12</v>
       </c>
       <c r="B132" s="15" t="s">
-        <v>79</v>
+        <v>74</v>
       </c>
       <c r="E132" s="10" t="s">
-        <v>219</v>
+        <v>213</v>
       </c>
     </row>
     <row r="133" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A133" s="23" t="s">
         <v>12</v>
       </c>
-      <c r="B133" s="16" t="s">
-        <v>77</v>
+      <c r="B133" s="15" t="s">
+        <v>75</v>
       </c>
       <c r="E133" s="10" t="s">
-        <v>220</v>
-      </c>
-    </row>
-    <row r="134" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="134" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A134" s="23" t="s">
         <v>12</v>
       </c>
-      <c r="B134" s="16" t="s">
-        <v>80</v>
-      </c>
-      <c r="C134" s="7" t="s">
-        <v>85</v>
+      <c r="B134" s="15" t="s">
+        <v>76</v>
       </c>
       <c r="E134" s="10" t="s">
-        <v>221</v>
-      </c>
-    </row>
-    <row r="135" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="135" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A135" s="23" t="s">
         <v>12</v>
       </c>
-      <c r="B135" s="16" t="s">
-        <v>81</v>
+      <c r="B135" s="15" t="s">
+        <v>78</v>
       </c>
       <c r="E135" s="10" t="s">
-        <v>222</v>
+        <v>216</v>
       </c>
     </row>
     <row r="136" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A136" s="23" t="s">
         <v>12</v>
       </c>
-      <c r="B136" s="16" t="s">
-        <v>82</v>
-      </c>
-      <c r="E136" s="10" t="s">
-        <v>223</v>
-      </c>
-    </row>
-    <row r="137" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="B136" s="15" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="137" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A137" s="23" t="s">
         <v>12</v>
       </c>
       <c r="B137" s="16" t="s">
-        <v>71</v>
+        <v>77</v>
       </c>
       <c r="E137" s="10" t="s">
-        <v>224</v>
+        <v>218</v>
       </c>
     </row>
     <row r="138" spans="1:5" ht="45" x14ac:dyDescent="0.25">
@@ -5381,111 +6530,128 @@
         <v>12</v>
       </c>
       <c r="B138" s="16" t="s">
-        <v>73</v>
+        <v>80</v>
+      </c>
+      <c r="C138" s="7" t="s">
+        <v>85</v>
       </c>
       <c r="E138" s="10" t="s">
-        <v>225</v>
+        <v>219</v>
       </c>
     </row>
     <row r="139" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A139" s="23" t="s">
         <v>12</v>
       </c>
-      <c r="B139" s="10" t="s">
-        <v>210</v>
+      <c r="B139" s="16" t="s">
+        <v>81</v>
       </c>
       <c r="E139" s="10" t="s">
-        <v>226</v>
-      </c>
-    </row>
-    <row r="140" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="140" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A140" s="23" t="s">
         <v>12</v>
       </c>
-      <c r="B140" s="22"/>
+      <c r="B140" s="16" t="s">
+        <v>82</v>
+      </c>
       <c r="E140" s="10" t="s">
-        <v>227</v>
+        <v>221</v>
       </c>
     </row>
     <row r="141" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A141" s="23" t="s">
         <v>12</v>
       </c>
-      <c r="B141" s="22"/>
+      <c r="B141" s="16" t="s">
+        <v>71</v>
+      </c>
       <c r="E141" s="10" t="s">
-        <v>228</v>
-      </c>
-    </row>
-    <row r="142" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="142" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A142" s="23" t="s">
         <v>12</v>
       </c>
-      <c r="B142" s="22"/>
+      <c r="B142" s="16" t="s">
+        <v>73</v>
+      </c>
       <c r="E142" s="10" t="s">
-        <v>229</v>
+        <v>223</v>
       </c>
     </row>
     <row r="143" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A143" s="23" t="s">
         <v>12</v>
       </c>
-      <c r="B143" s="22"/>
+      <c r="B143" s="16" t="s">
+        <v>210</v>
+      </c>
       <c r="E143" s="10" t="s">
-        <v>230</v>
+        <v>224</v>
       </c>
     </row>
     <row r="144" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A144" s="23" t="s">
         <v>12</v>
       </c>
-      <c r="B144" s="22"/>
-      <c r="E144" s="10" t="s">
-        <v>231</v>
+      <c r="B144" s="16" t="s">
+        <v>245</v>
       </c>
     </row>
     <row r="145" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A145" s="23" t="s">
         <v>12</v>
       </c>
-      <c r="B145" s="22"/>
+      <c r="B145" s="16" t="s">
+        <v>249</v>
+      </c>
       <c r="E145" s="10" t="s">
-        <v>232</v>
+        <v>226</v>
       </c>
     </row>
     <row r="146" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A146" s="23" t="s">
         <v>12</v>
       </c>
-      <c r="B146" s="22"/>
-      <c r="E146" s="10" t="s">
-        <v>233</v>
+      <c r="B146" s="55" t="s">
+        <v>217</v>
       </c>
     </row>
     <row r="147" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A147" s="23" t="s">
         <v>12</v>
       </c>
-      <c r="B147" s="22"/>
+      <c r="B147" s="55" t="s">
+        <v>225</v>
+      </c>
       <c r="E147" s="10" t="s">
-        <v>234</v>
+        <v>228</v>
       </c>
     </row>
     <row r="148" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A148" s="23" t="s">
         <v>12</v>
       </c>
-      <c r="B148" s="22"/>
+      <c r="B148" s="55" t="s">
+        <v>227</v>
+      </c>
       <c r="E148" s="10" t="s">
-        <v>235</v>
+        <v>229</v>
       </c>
     </row>
     <row r="149" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A149" s="23" t="s">
         <v>12</v>
       </c>
-      <c r="B149" s="22"/>
+      <c r="B149" s="22" t="s">
+        <v>253</v>
+      </c>
       <c r="E149" s="10" t="s">
-        <v>236</v>
+        <v>230</v>
       </c>
     </row>
     <row r="150" spans="1:5" ht="30" x14ac:dyDescent="0.25">
@@ -5494,17 +6660,15 @@
       </c>
       <c r="B150" s="22"/>
       <c r="E150" s="10" t="s">
-        <v>237</v>
-      </c>
-    </row>
-    <row r="151" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="151" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A151" s="23" t="s">
         <v>12</v>
       </c>
       <c r="B151" s="22"/>
-      <c r="E151" s="10" t="s">
-        <v>238</v>
-      </c>
+      <c r="E151" s="10"/>
     </row>
     <row r="152" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A152" s="23" t="s">
@@ -5512,21 +6676,57 @@
       </c>
       <c r="B152" s="22"/>
       <c r="E152" s="10" t="s">
-        <v>239</v>
+        <v>232</v>
+      </c>
+    </row>
+    <row r="153" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A153" s="23" t="s">
+        <v>12</v>
+      </c>
+      <c r="B153" s="22"/>
+      <c r="E153" s="10" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="154" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A154" s="23" t="s">
+        <v>12</v>
+      </c>
+      <c r="B154" s="22"/>
+      <c r="E154" s="10" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="155" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A155" s="23" t="s">
+        <v>12</v>
+      </c>
+      <c r="B155" s="22"/>
+      <c r="E155" s="10" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="156" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A156" s="23" t="s">
+        <v>12</v>
+      </c>
+      <c r="B156" s="22"/>
+      <c r="E156" s="10" t="s">
+        <v>236</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="C3" location="'ESC-CAL-0001-Seguridad'!A1" display="ESC-CAL-0001-Seguridad" xr:uid="{8C3432AC-6914-4481-A87B-E3FCB55DEAF8}"/>
     <hyperlink ref="C4" location="'ESC-CAL-0002-Seguridad'!A1" display="ESC-CAL-0002-Seguridad" xr:uid="{601180A6-524D-461A-8794-788E914D760E}"/>
-    <hyperlink ref="C33" location="'ESC-CAL-0001-Disponibilidad'!A1" display="ESC-CAL-0001-Disponibilidad" xr:uid="{FB125A2C-06EE-4D33-A57D-1D811EE4312A}"/>
-    <hyperlink ref="C34" location="'ESC-CAL-0002-Disponibilidad'!A1" display="ESC-CAL-0002-Disponibilidad" xr:uid="{ACE665FD-C5EF-4797-B9B9-8EF35659C63A}"/>
-    <hyperlink ref="C63" location="'ESC-CAL-0001-Portabilidad '!A1" display="ESC-CAL-0001-Portabilidad " xr:uid="{AAA89356-E1D1-45EA-8E3B-A0D1DD15F411}"/>
-    <hyperlink ref="C64" location="'ESC-CAL-0002-Portabilidad '!A1" display="ESC-CAL-0002-Portabilidad " xr:uid="{DECBCB46-A365-4C31-83AD-6D52A9D3E712}"/>
-    <hyperlink ref="C93" location="'ESC-CAL-0001-Eficiencia '!A1" display="ESC-CAL-0001-Eficiencia " xr:uid="{080A8C12-7DBD-4BC8-B0BA-E12C356590E3}"/>
-    <hyperlink ref="C94" location="'ESC-CAL-0002-Eficiencia '!A1" display="ESC-CAL-0002-Eficiencia " xr:uid="{C27C6FEF-D981-468E-896E-BCF9020357B2}"/>
-    <hyperlink ref="C123" location="'ESC-CAL-0001-Capacidad-Auditado'!A1" display="ESC-CAL-0001-Capacidad-Auditado " xr:uid="{08FE87C5-3371-430E-8C34-E03AF96DEF90}"/>
-    <hyperlink ref="C124" location="'ESC-CAL-0002-Capacidad-Auditado'!A1" display="ESC-CAL-0002-Capacidad-Auditado " xr:uid="{6DBE3107-E106-4314-83C2-E807D57AE5AC}"/>
+    <hyperlink ref="C37" location="'ESC-CAL-0001-Disponibilidad'!A1" display="ESC-CAL-0001-Disponibilidad" xr:uid="{FB125A2C-06EE-4D33-A57D-1D811EE4312A}"/>
+    <hyperlink ref="C38" location="'ESC-CAL-0002-Disponibilidad'!A1" display="ESC-CAL-0002-Disponibilidad" xr:uid="{ACE665FD-C5EF-4797-B9B9-8EF35659C63A}"/>
+    <hyperlink ref="C67" location="'ESC-CAL-0001-Portabilidad '!A1" display="ESC-CAL-0001-Portabilidad " xr:uid="{AAA89356-E1D1-45EA-8E3B-A0D1DD15F411}"/>
+    <hyperlink ref="C68" location="'ESC-CAL-0002-Portabilidad '!A1" display="ESC-CAL-0002-Portabilidad " xr:uid="{DECBCB46-A365-4C31-83AD-6D52A9D3E712}"/>
+    <hyperlink ref="C97" location="'ESC-CAL-0001-Eficiencia '!A1" display="ESC-CAL-0001-Eficiencia " xr:uid="{080A8C12-7DBD-4BC8-B0BA-E12C356590E3}"/>
+    <hyperlink ref="C98" location="'ESC-CAL-0002-Eficiencia '!A1" display="ESC-CAL-0002-Eficiencia " xr:uid="{C27C6FEF-D981-468E-896E-BCF9020357B2}"/>
+    <hyperlink ref="C127" location="'ESC-CAL-0001-Capacidad-Auditado'!A1" display="ESC-CAL-0001-Capacidad-Auditado " xr:uid="{08FE87C5-3371-430E-8C34-E03AF96DEF90}"/>
+    <hyperlink ref="C128" location="'ESC-CAL-0002-Capacidad-Auditado'!A1" display="ESC-CAL-0002-Capacidad-Auditado " xr:uid="{6DBE3107-E106-4314-83C2-E807D57AE5AC}"/>
     <hyperlink ref="A1" location="'Tabla de Contenido'!A1" display="Tabla de Contenido" xr:uid="{B1F41128-BC2A-499D-BC6D-56C34EB084DA}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -5536,7 +6736,7 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E9A4312C-FDD2-4340-821F-754A5F40D4E6}">
-  <dimension ref="A1:I7"/>
+  <dimension ref="A1:I15"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -5608,9 +6808,125 @@
         <v>147</v>
       </c>
     </row>
+    <row r="12" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+      <c r="A12" s="54" t="s">
+        <v>112</v>
+      </c>
+      <c r="B12" s="54" t="s">
+        <v>113</v>
+      </c>
+      <c r="C12" s="54" t="s">
+        <v>114</v>
+      </c>
+      <c r="D12" s="54" t="s">
+        <v>115</v>
+      </c>
+      <c r="E12" s="54" t="s">
+        <v>116</v>
+      </c>
+      <c r="F12" s="54" t="s">
+        <v>117</v>
+      </c>
+      <c r="G12" s="54" t="s">
+        <v>118</v>
+      </c>
+      <c r="H12" s="54" t="s">
+        <v>119</v>
+      </c>
+      <c r="I12" s="54" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" ht="210" x14ac:dyDescent="0.25">
+      <c r="A13" s="10">
+        <v>1</v>
+      </c>
+      <c r="B13" s="10" t="s">
+        <v>400</v>
+      </c>
+      <c r="C13" s="10" t="s">
+        <v>122</v>
+      </c>
+      <c r="D13" s="10" t="s">
+        <v>401</v>
+      </c>
+      <c r="E13" s="10" t="s">
+        <v>263</v>
+      </c>
+      <c r="F13" s="10" t="s">
+        <v>125</v>
+      </c>
+      <c r="G13" s="10" t="s">
+        <v>402</v>
+      </c>
+      <c r="H13" s="10" t="s">
+        <v>403</v>
+      </c>
+      <c r="I13" s="10" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" ht="255" x14ac:dyDescent="0.25">
+      <c r="A14" s="10">
+        <v>2</v>
+      </c>
+      <c r="B14" s="10" t="s">
+        <v>404</v>
+      </c>
+      <c r="C14" s="10" t="s">
+        <v>405</v>
+      </c>
+      <c r="D14" s="10" t="s">
+        <v>406</v>
+      </c>
+      <c r="E14" s="10" t="s">
+        <v>263</v>
+      </c>
+      <c r="F14" s="10" t="s">
+        <v>125</v>
+      </c>
+      <c r="G14" s="10" t="s">
+        <v>407</v>
+      </c>
+      <c r="H14" s="10" t="s">
+        <v>408</v>
+      </c>
+      <c r="I14" s="10" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" ht="180" x14ac:dyDescent="0.25">
+      <c r="A15" s="10">
+        <v>3</v>
+      </c>
+      <c r="B15" s="10" t="s">
+        <v>409</v>
+      </c>
+      <c r="C15" s="10" t="s">
+        <v>122</v>
+      </c>
+      <c r="D15" s="10" t="s">
+        <v>410</v>
+      </c>
+      <c r="E15" s="10" t="s">
+        <v>263</v>
+      </c>
+      <c r="F15" s="10" t="s">
+        <v>125</v>
+      </c>
+      <c r="G15" s="10" t="s">
+        <v>411</v>
+      </c>
+      <c r="H15" s="10" t="s">
+        <v>412</v>
+      </c>
+      <c r="I15" s="10" t="s">
+        <v>128</v>
+      </c>
+    </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="A1" location="Caracterizacion!A1" display="Caracterizacion" xr:uid="{4143DDCD-F253-4DA2-9589-F65532AB8B6D}"/>
+    <hyperlink ref="A1" location="Caracterizacion!A127" display="Caracterizacion" xr:uid="{4143DDCD-F253-4DA2-9589-F65532AB8B6D}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -5618,7 +6934,7 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0B71487E-C9E1-4276-81FB-A1C49393F747}">
-  <dimension ref="A1:I7"/>
+  <dimension ref="A1:I15"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -5690,9 +7006,128 @@
         <v>147</v>
       </c>
     </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B10" s="6"/>
+    </row>
+    <row r="12" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+      <c r="A12" s="54" t="s">
+        <v>112</v>
+      </c>
+      <c r="B12" s="54" t="s">
+        <v>113</v>
+      </c>
+      <c r="C12" s="54" t="s">
+        <v>114</v>
+      </c>
+      <c r="D12" s="54" t="s">
+        <v>115</v>
+      </c>
+      <c r="E12" s="54" t="s">
+        <v>116</v>
+      </c>
+      <c r="F12" s="54" t="s">
+        <v>117</v>
+      </c>
+      <c r="G12" s="54" t="s">
+        <v>118</v>
+      </c>
+      <c r="H12" s="54" t="s">
+        <v>119</v>
+      </c>
+      <c r="I12" s="54" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" ht="150" x14ac:dyDescent="0.25">
+      <c r="A13" s="10">
+        <v>1</v>
+      </c>
+      <c r="B13" s="10" t="s">
+        <v>413</v>
+      </c>
+      <c r="C13" s="10" t="s">
+        <v>405</v>
+      </c>
+      <c r="D13" s="10" t="s">
+        <v>414</v>
+      </c>
+      <c r="E13" s="10" t="s">
+        <v>263</v>
+      </c>
+      <c r="F13" s="10" t="s">
+        <v>125</v>
+      </c>
+      <c r="G13" s="10" t="s">
+        <v>415</v>
+      </c>
+      <c r="H13" s="10" t="s">
+        <v>416</v>
+      </c>
+      <c r="I13" s="10" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" ht="210" x14ac:dyDescent="0.25">
+      <c r="A14" s="10">
+        <v>2</v>
+      </c>
+      <c r="B14" s="10" t="s">
+        <v>417</v>
+      </c>
+      <c r="C14" s="10" t="s">
+        <v>405</v>
+      </c>
+      <c r="D14" s="10" t="s">
+        <v>418</v>
+      </c>
+      <c r="E14" s="10" t="s">
+        <v>263</v>
+      </c>
+      <c r="F14" s="10" t="s">
+        <v>125</v>
+      </c>
+      <c r="G14" s="10" t="s">
+        <v>419</v>
+      </c>
+      <c r="H14" s="10" t="s">
+        <v>420</v>
+      </c>
+      <c r="I14" s="10" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" ht="150" x14ac:dyDescent="0.25">
+      <c r="A15" s="10">
+        <v>3</v>
+      </c>
+      <c r="B15" s="10" t="s">
+        <v>421</v>
+      </c>
+      <c r="C15" s="10" t="s">
+        <v>405</v>
+      </c>
+      <c r="D15" s="10" t="s">
+        <v>422</v>
+      </c>
+      <c r="E15" s="10" t="s">
+        <v>263</v>
+      </c>
+      <c r="F15" s="10" t="s">
+        <v>125</v>
+      </c>
+      <c r="G15" s="10" t="s">
+        <v>423</v>
+      </c>
+      <c r="H15" s="10" t="s">
+        <v>424</v>
+      </c>
+      <c r="I15" s="10" t="s">
+        <v>128</v>
+      </c>
+    </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="A1" location="Caracterizacion!A1" display="Caracterizacion" xr:uid="{25DF7DEB-8E86-49F3-8F50-653C867B0F13}"/>
+    <hyperlink ref="A1" location="Caracterizacion!A127" display="Caracterizacion" xr:uid="{25DF7DEB-8E86-49F3-8F50-653C867B0F13}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -5700,7 +7135,7 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{482B083A-8F1B-4380-B3DA-4DA002A053C1}">
-  <dimension ref="A1:I7"/>
+  <dimension ref="A1:I13"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -5772,9 +7207,125 @@
         <v>147</v>
       </c>
     </row>
+    <row r="10" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+      <c r="A10" s="54" t="s">
+        <v>112</v>
+      </c>
+      <c r="B10" s="54" t="s">
+        <v>113</v>
+      </c>
+      <c r="C10" s="54" t="s">
+        <v>114</v>
+      </c>
+      <c r="D10" s="54" t="s">
+        <v>115</v>
+      </c>
+      <c r="E10" s="54" t="s">
+        <v>116</v>
+      </c>
+      <c r="F10" s="54" t="s">
+        <v>117</v>
+      </c>
+      <c r="G10" s="54" t="s">
+        <v>118</v>
+      </c>
+      <c r="H10" s="54" t="s">
+        <v>119</v>
+      </c>
+      <c r="I10" s="54" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" ht="165" x14ac:dyDescent="0.25">
+      <c r="A11" s="10">
+        <v>1</v>
+      </c>
+      <c r="B11" s="10" t="s">
+        <v>378</v>
+      </c>
+      <c r="C11" s="10" t="s">
+        <v>122</v>
+      </c>
+      <c r="D11" s="10" t="s">
+        <v>379</v>
+      </c>
+      <c r="E11" s="10" t="s">
+        <v>263</v>
+      </c>
+      <c r="F11" s="10" t="s">
+        <v>125</v>
+      </c>
+      <c r="G11" s="10" t="s">
+        <v>380</v>
+      </c>
+      <c r="H11" s="10" t="s">
+        <v>381</v>
+      </c>
+      <c r="I11" s="10" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" ht="285" x14ac:dyDescent="0.25">
+      <c r="A12" s="10">
+        <v>2</v>
+      </c>
+      <c r="B12" s="10" t="s">
+        <v>382</v>
+      </c>
+      <c r="C12" s="10" t="s">
+        <v>122</v>
+      </c>
+      <c r="D12" s="10" t="s">
+        <v>383</v>
+      </c>
+      <c r="E12" s="10" t="s">
+        <v>263</v>
+      </c>
+      <c r="F12" s="10" t="s">
+        <v>125</v>
+      </c>
+      <c r="G12" s="10" t="s">
+        <v>384</v>
+      </c>
+      <c r="H12" s="10" t="s">
+        <v>385</v>
+      </c>
+      <c r="I12" s="10" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" ht="255" x14ac:dyDescent="0.25">
+      <c r="A13" s="10">
+        <v>3</v>
+      </c>
+      <c r="B13" s="10" t="s">
+        <v>386</v>
+      </c>
+      <c r="C13" s="10" t="s">
+        <v>122</v>
+      </c>
+      <c r="D13" s="10" t="s">
+        <v>387</v>
+      </c>
+      <c r="E13" s="10" t="s">
+        <v>263</v>
+      </c>
+      <c r="F13" s="10" t="s">
+        <v>125</v>
+      </c>
+      <c r="G13" s="10" t="s">
+        <v>388</v>
+      </c>
+      <c r="H13" s="10" t="s">
+        <v>381</v>
+      </c>
+      <c r="I13" s="10" t="s">
+        <v>128</v>
+      </c>
+    </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="A1" location="Caracterizacion!A1" display="Caracterizacion" xr:uid="{9A883409-1D3F-40C4-BA5A-17A4D12C8197}"/>
+    <hyperlink ref="A1" location="Caracterizacion!A97" display="Caracterizacion" xr:uid="{9A883409-1D3F-40C4-BA5A-17A4D12C8197}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -5782,7 +7333,7 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FA19D2B3-3E99-4B9E-BAE1-41A4FFCD985E}">
-  <dimension ref="A1:I7"/>
+  <dimension ref="A1:I14"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -5854,9 +7405,125 @@
         <v>147</v>
       </c>
     </row>
+    <row r="11" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+      <c r="A11" s="54" t="s">
+        <v>112</v>
+      </c>
+      <c r="B11" s="54" t="s">
+        <v>113</v>
+      </c>
+      <c r="C11" s="54" t="s">
+        <v>114</v>
+      </c>
+      <c r="D11" s="54" t="s">
+        <v>115</v>
+      </c>
+      <c r="E11" s="54" t="s">
+        <v>116</v>
+      </c>
+      <c r="F11" s="54" t="s">
+        <v>117</v>
+      </c>
+      <c r="G11" s="54" t="s">
+        <v>118</v>
+      </c>
+      <c r="H11" s="54" t="s">
+        <v>119</v>
+      </c>
+      <c r="I11" s="54" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" ht="165" x14ac:dyDescent="0.25">
+      <c r="A12" s="10">
+        <v>1</v>
+      </c>
+      <c r="B12" s="10" t="s">
+        <v>389</v>
+      </c>
+      <c r="C12" s="10" t="s">
+        <v>122</v>
+      </c>
+      <c r="D12" s="10" t="s">
+        <v>390</v>
+      </c>
+      <c r="E12" s="10" t="s">
+        <v>263</v>
+      </c>
+      <c r="F12" s="10" t="s">
+        <v>125</v>
+      </c>
+      <c r="G12" s="10" t="s">
+        <v>391</v>
+      </c>
+      <c r="H12" s="10" t="s">
+        <v>392</v>
+      </c>
+      <c r="I12" s="10" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" ht="285" x14ac:dyDescent="0.25">
+      <c r="A13" s="10">
+        <v>2</v>
+      </c>
+      <c r="B13" s="10" t="s">
+        <v>393</v>
+      </c>
+      <c r="C13" s="10" t="s">
+        <v>122</v>
+      </c>
+      <c r="D13" s="10" t="s">
+        <v>394</v>
+      </c>
+      <c r="E13" s="10" t="s">
+        <v>263</v>
+      </c>
+      <c r="F13" s="10" t="s">
+        <v>125</v>
+      </c>
+      <c r="G13" s="10" t="s">
+        <v>395</v>
+      </c>
+      <c r="H13" s="10" t="s">
+        <v>396</v>
+      </c>
+      <c r="I13" s="10" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" ht="255" x14ac:dyDescent="0.25">
+      <c r="A14" s="10">
+        <v>3</v>
+      </c>
+      <c r="B14" s="10" t="s">
+        <v>397</v>
+      </c>
+      <c r="C14" s="10" t="s">
+        <v>122</v>
+      </c>
+      <c r="D14" s="10" t="s">
+        <v>398</v>
+      </c>
+      <c r="E14" s="10" t="s">
+        <v>263</v>
+      </c>
+      <c r="F14" s="10" t="s">
+        <v>125</v>
+      </c>
+      <c r="G14" s="10" t="s">
+        <v>399</v>
+      </c>
+      <c r="H14" s="10" t="s">
+        <v>392</v>
+      </c>
+      <c r="I14" s="10" t="s">
+        <v>128</v>
+      </c>
+    </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="A1" location="Caracterizacion!A1" display="Caracterizacion" xr:uid="{1156F991-BF1F-400B-8E45-721113686811}"/>
+    <hyperlink ref="A1" location="Caracterizacion!A97" display="Caracterizacion" xr:uid="{1156F991-BF1F-400B-8E45-721113686811}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -5864,7 +7531,7 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{77AFA58C-0D37-472A-9044-2D31A2B22101}">
-  <dimension ref="A1:I7"/>
+  <dimension ref="A1:I14"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -5936,9 +7603,125 @@
         <v>147</v>
       </c>
     </row>
+    <row r="11" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+      <c r="A11" s="54" t="s">
+        <v>112</v>
+      </c>
+      <c r="B11" s="54" t="s">
+        <v>113</v>
+      </c>
+      <c r="C11" s="54" t="s">
+        <v>311</v>
+      </c>
+      <c r="D11" s="54" t="s">
+        <v>115</v>
+      </c>
+      <c r="E11" s="54" t="s">
+        <v>116</v>
+      </c>
+      <c r="F11" s="54" t="s">
+        <v>117</v>
+      </c>
+      <c r="G11" s="54" t="s">
+        <v>118</v>
+      </c>
+      <c r="H11" s="54" t="s">
+        <v>312</v>
+      </c>
+      <c r="I11" s="54" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" ht="150" x14ac:dyDescent="0.25">
+      <c r="A12" s="10">
+        <v>1</v>
+      </c>
+      <c r="B12" s="10" t="s">
+        <v>346</v>
+      </c>
+      <c r="C12" s="10" t="s">
+        <v>122</v>
+      </c>
+      <c r="D12" s="10" t="s">
+        <v>347</v>
+      </c>
+      <c r="E12" s="10" t="s">
+        <v>124</v>
+      </c>
+      <c r="F12" s="10" t="s">
+        <v>348</v>
+      </c>
+      <c r="G12" s="10" t="s">
+        <v>349</v>
+      </c>
+      <c r="H12" s="10" t="s">
+        <v>350</v>
+      </c>
+      <c r="I12" s="10" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" ht="195" x14ac:dyDescent="0.25">
+      <c r="A13" s="10">
+        <v>2</v>
+      </c>
+      <c r="B13" s="10" t="s">
+        <v>351</v>
+      </c>
+      <c r="C13" s="10" t="s">
+        <v>122</v>
+      </c>
+      <c r="D13" s="10" t="s">
+        <v>352</v>
+      </c>
+      <c r="E13" s="10" t="s">
+        <v>124</v>
+      </c>
+      <c r="F13" s="10" t="s">
+        <v>353</v>
+      </c>
+      <c r="G13" s="10" t="s">
+        <v>354</v>
+      </c>
+      <c r="H13" s="10" t="s">
+        <v>355</v>
+      </c>
+      <c r="I13" s="10" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" ht="180" x14ac:dyDescent="0.25">
+      <c r="A14" s="10">
+        <v>3</v>
+      </c>
+      <c r="B14" s="10" t="s">
+        <v>356</v>
+      </c>
+      <c r="C14" s="10" t="s">
+        <v>122</v>
+      </c>
+      <c r="D14" s="10" t="s">
+        <v>357</v>
+      </c>
+      <c r="E14" s="10" t="s">
+        <v>124</v>
+      </c>
+      <c r="F14" s="10" t="s">
+        <v>358</v>
+      </c>
+      <c r="G14" s="10" t="s">
+        <v>359</v>
+      </c>
+      <c r="H14" s="10" t="s">
+        <v>360</v>
+      </c>
+      <c r="I14" s="10" t="s">
+        <v>128</v>
+      </c>
+    </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="A1" location="Caracterizacion!A1" display="Caracterizacion" xr:uid="{17B41008-2528-4E09-9F07-0866EB53A867}"/>
+    <hyperlink ref="A1" location="Caracterizacion!A67" display="Caracterizacion" xr:uid="{17B41008-2528-4E09-9F07-0866EB53A867}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -5946,7 +7729,7 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9BF74A5E-2AA8-4C93-B20D-32544E95EFB7}">
-  <dimension ref="A1:I7"/>
+  <dimension ref="A1:I16"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -6018,9 +7801,125 @@
         <v>147</v>
       </c>
     </row>
+    <row r="13" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+      <c r="A13" s="54" t="s">
+        <v>112</v>
+      </c>
+      <c r="B13" s="54" t="s">
+        <v>113</v>
+      </c>
+      <c r="C13" s="54" t="s">
+        <v>311</v>
+      </c>
+      <c r="D13" s="54" t="s">
+        <v>115</v>
+      </c>
+      <c r="E13" s="54" t="s">
+        <v>116</v>
+      </c>
+      <c r="F13" s="54" t="s">
+        <v>117</v>
+      </c>
+      <c r="G13" s="54" t="s">
+        <v>118</v>
+      </c>
+      <c r="H13" s="54" t="s">
+        <v>312</v>
+      </c>
+      <c r="I13" s="54" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" ht="210" x14ac:dyDescent="0.25">
+      <c r="A14" s="10">
+        <v>1</v>
+      </c>
+      <c r="B14" s="10" t="s">
+        <v>361</v>
+      </c>
+      <c r="C14" s="10" t="s">
+        <v>122</v>
+      </c>
+      <c r="D14" s="10" t="s">
+        <v>362</v>
+      </c>
+      <c r="E14" s="10" t="s">
+        <v>124</v>
+      </c>
+      <c r="F14" s="10" t="s">
+        <v>363</v>
+      </c>
+      <c r="G14" s="10" t="s">
+        <v>364</v>
+      </c>
+      <c r="H14" s="10" t="s">
+        <v>365</v>
+      </c>
+      <c r="I14" s="10" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" ht="210" x14ac:dyDescent="0.25">
+      <c r="A15" s="10">
+        <v>2</v>
+      </c>
+      <c r="B15" s="10" t="s">
+        <v>366</v>
+      </c>
+      <c r="C15" s="10" t="s">
+        <v>122</v>
+      </c>
+      <c r="D15" s="10" t="s">
+        <v>367</v>
+      </c>
+      <c r="E15" s="10" t="s">
+        <v>124</v>
+      </c>
+      <c r="F15" s="10" t="s">
+        <v>363</v>
+      </c>
+      <c r="G15" s="10" t="s">
+        <v>368</v>
+      </c>
+      <c r="H15" s="10" t="s">
+        <v>369</v>
+      </c>
+      <c r="I15" s="10" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" ht="180" x14ac:dyDescent="0.25">
+      <c r="A16" s="10">
+        <v>3</v>
+      </c>
+      <c r="B16" s="10" t="s">
+        <v>370</v>
+      </c>
+      <c r="C16" s="10" t="s">
+        <v>122</v>
+      </c>
+      <c r="D16" s="10" t="s">
+        <v>371</v>
+      </c>
+      <c r="E16" s="10" t="s">
+        <v>124</v>
+      </c>
+      <c r="F16" s="10" t="s">
+        <v>372</v>
+      </c>
+      <c r="G16" s="10" t="s">
+        <v>373</v>
+      </c>
+      <c r="H16" s="10" t="s">
+        <v>374</v>
+      </c>
+      <c r="I16" s="10" t="s">
+        <v>128</v>
+      </c>
+    </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="A1" location="Caracterizacion!A1" display="Caracterizacion" xr:uid="{6F08598B-8F31-453A-BCEF-311AF3C6193A}"/>
+    <hyperlink ref="A1" location="Caracterizacion!A67" display="Caracterizacion" xr:uid="{6F08598B-8F31-453A-BCEF-311AF3C6193A}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -6028,7 +7927,7 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4AABED7F-A641-414C-93D1-501EE24037CE}">
-  <dimension ref="A1:I7"/>
+  <dimension ref="A1:I16"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -6100,9 +7999,125 @@
         <v>147</v>
       </c>
     </row>
+    <row r="13" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+      <c r="A13" s="54" t="s">
+        <v>112</v>
+      </c>
+      <c r="B13" s="54" t="s">
+        <v>113</v>
+      </c>
+      <c r="C13" s="54" t="s">
+        <v>311</v>
+      </c>
+      <c r="D13" s="54" t="s">
+        <v>115</v>
+      </c>
+      <c r="E13" s="54" t="s">
+        <v>116</v>
+      </c>
+      <c r="F13" s="54" t="s">
+        <v>117</v>
+      </c>
+      <c r="G13" s="54" t="s">
+        <v>118</v>
+      </c>
+      <c r="H13" s="54" t="s">
+        <v>312</v>
+      </c>
+      <c r="I13" s="54" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" ht="150" x14ac:dyDescent="0.25">
+      <c r="A14" s="10">
+        <v>1</v>
+      </c>
+      <c r="B14" s="10" t="s">
+        <v>313</v>
+      </c>
+      <c r="C14" s="10" t="s">
+        <v>314</v>
+      </c>
+      <c r="D14" s="10" t="s">
+        <v>315</v>
+      </c>
+      <c r="E14" s="10" t="s">
+        <v>124</v>
+      </c>
+      <c r="F14" s="10" t="s">
+        <v>264</v>
+      </c>
+      <c r="G14" s="10" t="s">
+        <v>316</v>
+      </c>
+      <c r="H14" s="10" t="s">
+        <v>317</v>
+      </c>
+      <c r="I14" s="10" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" ht="195" x14ac:dyDescent="0.25">
+      <c r="A15" s="10">
+        <v>2</v>
+      </c>
+      <c r="B15" s="10" t="s">
+        <v>318</v>
+      </c>
+      <c r="C15" s="10" t="s">
+        <v>319</v>
+      </c>
+      <c r="D15" s="10" t="s">
+        <v>320</v>
+      </c>
+      <c r="E15" s="10" t="s">
+        <v>124</v>
+      </c>
+      <c r="F15" s="10" t="s">
+        <v>264</v>
+      </c>
+      <c r="G15" s="10" t="s">
+        <v>321</v>
+      </c>
+      <c r="H15" s="10" t="s">
+        <v>322</v>
+      </c>
+      <c r="I15" s="10" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" ht="210" x14ac:dyDescent="0.25">
+      <c r="A16" s="10">
+        <v>3</v>
+      </c>
+      <c r="B16" s="10" t="s">
+        <v>323</v>
+      </c>
+      <c r="C16" s="10" t="s">
+        <v>324</v>
+      </c>
+      <c r="D16" s="10" t="s">
+        <v>325</v>
+      </c>
+      <c r="E16" s="10" t="s">
+        <v>124</v>
+      </c>
+      <c r="F16" s="10" t="s">
+        <v>264</v>
+      </c>
+      <c r="G16" s="10" t="s">
+        <v>326</v>
+      </c>
+      <c r="H16" s="10" t="s">
+        <v>327</v>
+      </c>
+      <c r="I16" s="10" t="s">
+        <v>128</v>
+      </c>
+    </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="A1" location="Caracterizacion!A1" display="Caracterizacion" xr:uid="{3CEF3482-DDF5-411B-9567-0C954DF9038A}"/>
+    <hyperlink ref="A1" location="Caracterizacion!A37" display="Caracterizacion" xr:uid="{3CEF3482-DDF5-411B-9567-0C954DF9038A}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>